<commit_message>
Fix values for public health in data; Added axes
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="13">
   <si>
     <t>Hospitals</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Public</t>
-  </si>
-  <si>
-    <t>---</t>
   </si>
 </sst>
 </file>
@@ -393,7 +390,7 @@
   <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -468,8 +465,8 @@
       <c r="G2" s="1">
         <v>5.5065331683550509</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
+      <c r="H2" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I2" s="1">
         <v>2.4902857796350717</v>
@@ -503,8 +500,8 @@
       <c r="G3" s="1">
         <v>5.4794851209165172</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
+      <c r="H3" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I3" s="1">
         <v>1.9186139464674519</v>
@@ -538,8 +535,8 @@
       <c r="G4" s="1">
         <v>4.9452337965621282</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>13</v>
+      <c r="H4" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I4" s="1">
         <v>2.5009727817632239</v>
@@ -573,8 +570,8 @@
       <c r="G5" s="1">
         <v>5.3461112372282358</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>13</v>
+      <c r="H5" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I5" s="1">
         <v>2.1189490729809384</v>
@@ -608,8 +605,8 @@
       <c r="G6" s="1">
         <v>3.8405144417463206</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>13</v>
+      <c r="H6" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I6" s="1">
         <v>2.1678166279218387</v>
@@ -643,8 +640,8 @@
       <c r="G7" s="1">
         <v>6.5141478370322501</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>13</v>
+      <c r="H7" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I7" s="1">
         <v>2.1462068275040491</v>
@@ -678,8 +675,8 @@
       <c r="G8" s="1">
         <v>5.9880057480333928</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>13</v>
+      <c r="H8" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I8" s="1">
         <v>2.9440603504534901</v>
@@ -713,8 +710,8 @@
       <c r="G9" s="1">
         <v>6.6892712306119746</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>13</v>
+      <c r="H9" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I9" s="1">
         <v>2.0054116046890318</v>
@@ -748,8 +745,8 @@
       <c r="G10" s="1">
         <v>4.6662077807147933</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>13</v>
+      <c r="H10" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I10" s="1">
         <v>2.1701122947580842</v>
@@ -783,8 +780,8 @@
       <c r="G11" s="1">
         <v>4.1457833058790481</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>13</v>
+      <c r="H11" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I11" s="1">
         <v>2.848502078816856</v>
@@ -818,8 +815,8 @@
       <c r="G12" s="1">
         <v>4.2512865365018744</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>13</v>
+      <c r="H12" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I12" s="1">
         <v>2.7623850584509517</v>
@@ -853,8 +850,8 @@
       <c r="G13" s="1">
         <v>4.162407053717585</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>13</v>
+      <c r="H13" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I13" s="1">
         <v>2.7420344922502262</v>
@@ -888,8 +885,8 @@
       <c r="G14" s="1">
         <v>4.0971305489195693</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>13</v>
+      <c r="H14" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I14" s="1">
         <v>2.3899259493951694</v>
@@ -923,8 +920,8 @@
       <c r="G15" s="1">
         <v>2.7430629868476473</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>13</v>
+      <c r="H15" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I15" s="1">
         <v>3.3311928089485932</v>
@@ -958,8 +955,8 @@
       <c r="G16" s="1">
         <v>2.7523041683721945</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>13</v>
+      <c r="H16" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I16" s="1">
         <v>4.6542852156779526</v>
@@ -993,8 +990,8 @@
       <c r="G17" s="1">
         <v>2.4611205370017868</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>13</v>
+      <c r="H17" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I17" s="1">
         <v>4.2715165308090546</v>
@@ -1028,8 +1025,8 @@
       <c r="G18" s="1">
         <v>2.0210962415748539</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>13</v>
+      <c r="H18" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I18" s="1">
         <v>4.4173485345120032</v>
@@ -1063,8 +1060,8 @@
       <c r="G19" s="1">
         <v>2.0047812775642835</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>13</v>
+      <c r="H19" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I19" s="1">
         <v>4.4445241495861367</v>
@@ -1098,8 +1095,8 @@
       <c r="G20" s="1">
         <v>1.8731439386793229</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>13</v>
+      <c r="H20" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I20" s="1">
         <v>5.4144292803451606</v>
@@ -1133,8 +1130,8 @@
       <c r="G21" s="1">
         <v>1.6022140836252803</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>13</v>
+      <c r="H21" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I21" s="1">
         <v>5.9606971911011959</v>
@@ -1168,8 +1165,8 @@
       <c r="G22" s="1">
         <v>2.0549475055926392</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>13</v>
+      <c r="H22" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I22" s="1">
         <v>5.9619596422091714</v>
@@ -1203,8 +1200,8 @@
       <c r="G23" s="1">
         <v>2.1635018667518442</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>13</v>
+      <c r="H23" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I23" s="1">
         <v>5.9745516029577912</v>
@@ -1238,8 +1235,8 @@
       <c r="G24" s="1">
         <v>1.5481777542137791</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>13</v>
+      <c r="H24" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I24" s="1">
         <v>5.487794975807283</v>
@@ -1273,8 +1270,8 @@
       <c r="G25" s="1">
         <v>1.7170139729484681</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>13</v>
+      <c r="H25" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I25" s="1">
         <v>4.4593898112558827</v>
@@ -1308,8 +1305,8 @@
       <c r="G26" s="1">
         <v>3.2453341512972078</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>13</v>
+      <c r="H26" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I26" s="1">
         <v>4.9051481990169776</v>
@@ -1343,8 +1340,8 @@
       <c r="G27" s="1">
         <v>2.8314295624156745</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>13</v>
+      <c r="H27" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I27" s="1">
         <v>5.1625159043856375</v>
@@ -1378,8 +1375,8 @@
       <c r="G28" s="1">
         <v>3.3796195901418034</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>13</v>
+      <c r="H28" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I28" s="1">
         <v>6.1772598553080611</v>
@@ -1413,8 +1410,8 @@
       <c r="G29" s="1">
         <v>3.5066708574563585</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>13</v>
+      <c r="H29" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I29" s="1">
         <v>6.556186894042658</v>
@@ -1448,8 +1445,8 @@
       <c r="G30" s="1">
         <v>3.8446688842753174</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>13</v>
+      <c r="H30" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I30" s="1">
         <v>7.0361815903898757</v>
@@ -1483,8 +1480,8 @@
       <c r="G31" s="1">
         <v>2.7816817381932761</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>13</v>
+      <c r="H31" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I31" s="1">
         <v>6.9546991199255546</v>
@@ -1518,8 +1515,8 @@
       <c r="G32" s="1">
         <v>3.5298957560305446</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>13</v>
+      <c r="H32" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I32" s="1">
         <v>6.2342441869814635</v>
@@ -1553,8 +1550,8 @@
       <c r="G33" s="1">
         <v>4.5002924041878627</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>13</v>
+      <c r="H33" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I33" s="1">
         <v>5.6493469322113503</v>
@@ -1588,8 +1585,8 @@
       <c r="G34" s="1">
         <v>3.246593360264499</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>13</v>
+      <c r="H34" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I34" s="1">
         <v>5.9353878829828908</v>
@@ -1623,8 +1620,8 @@
       <c r="G35" s="1">
         <v>2.777505457025887</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>13</v>
+      <c r="H35" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I35" s="1">
         <v>6.214280874782121</v>
@@ -1658,8 +1655,8 @@
       <c r="G36" s="1">
         <v>2.8656241961201157</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>13</v>
+      <c r="H36" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I36" s="1">
         <v>5.9263717750438145</v>
@@ -1693,8 +1690,8 @@
       <c r="G37" s="1">
         <v>3.602411802477627</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>13</v>
+      <c r="H37" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I37" s="1">
         <v>5.8610806676661307</v>
@@ -1728,8 +1725,8 @@
       <c r="G38" s="1">
         <v>3.4712443144576053</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>13</v>
+      <c r="H38" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I38" s="1">
         <v>6.2044998488071466</v>
@@ -1763,8 +1760,8 @@
       <c r="G39" s="1">
         <v>3.5701152246303116</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>13</v>
+      <c r="H39" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I39" s="1">
         <v>5.8334041434884281</v>
@@ -1798,8 +1795,8 @@
       <c r="G40" s="1">
         <v>2.254942260711331</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>13</v>
+      <c r="H40" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I40" s="1">
         <v>5.9712187990928589</v>
@@ -1833,8 +1830,8 @@
       <c r="G41" s="1">
         <v>2.7144899914682092</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>13</v>
+      <c r="H41" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I41" s="1">
         <v>5.7931576191024865</v>
@@ -1868,8 +1865,8 @@
       <c r="G42" s="1">
         <v>2.4421309148656056</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>13</v>
+      <c r="H42" s="1">
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="I42" s="1">
         <v>5.6530008904289835</v>

</xml_diff>

<commit_message>
Modified data series in attempt to make other filters work
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="15">
   <si>
     <t>Hospitals</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>Public</t>
+  </si>
+  <si>
+    <t>Private1</t>
+  </si>
+  <si>
+    <t>Public1</t>
   </si>
 </sst>
 </file>
@@ -387,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K83"/>
+  <dimension ref="A1:K165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="B125" sqref="B125:J165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -466,7 +472,7 @@
         <v>5.5065331683550509</v>
       </c>
       <c r="H2" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1">
         <v>2.4902857796350717</v>
@@ -501,7 +507,7 @@
         <v>5.4794851209165172</v>
       </c>
       <c r="H3" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1">
         <v>1.9186139464674519</v>
@@ -536,7 +542,7 @@
         <v>4.9452337965621282</v>
       </c>
       <c r="H4" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1">
         <v>2.5009727817632239</v>
@@ -571,7 +577,7 @@
         <v>5.3461112372282358</v>
       </c>
       <c r="H5" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1">
         <v>2.1189490729809384</v>
@@ -606,7 +612,7 @@
         <v>3.8405144417463206</v>
       </c>
       <c r="H6" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I6" s="1">
         <v>2.1678166279218387</v>
@@ -641,7 +647,7 @@
         <v>6.5141478370322501</v>
       </c>
       <c r="H7" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I7" s="1">
         <v>2.1462068275040491</v>
@@ -676,7 +682,7 @@
         <v>5.9880057480333928</v>
       </c>
       <c r="H8" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1">
         <v>2.9440603504534901</v>
@@ -711,7 +717,7 @@
         <v>6.6892712306119746</v>
       </c>
       <c r="H9" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1">
         <v>2.0054116046890318</v>
@@ -746,7 +752,7 @@
         <v>4.6662077807147933</v>
       </c>
       <c r="H10" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1">
         <v>2.1701122947580842</v>
@@ -781,7 +787,7 @@
         <v>4.1457833058790481</v>
       </c>
       <c r="H11" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I11" s="1">
         <v>2.848502078816856</v>
@@ -816,7 +822,7 @@
         <v>4.2512865365018744</v>
       </c>
       <c r="H12" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I12" s="1">
         <v>2.7623850584509517</v>
@@ -851,7 +857,7 @@
         <v>4.162407053717585</v>
       </c>
       <c r="H13" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I13" s="1">
         <v>2.7420344922502262</v>
@@ -886,7 +892,7 @@
         <v>4.0971305489195693</v>
       </c>
       <c r="H14" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I14" s="1">
         <v>2.3899259493951694</v>
@@ -921,7 +927,7 @@
         <v>2.7430629868476473</v>
       </c>
       <c r="H15" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I15" s="1">
         <v>3.3311928089485932</v>
@@ -956,7 +962,7 @@
         <v>2.7523041683721945</v>
       </c>
       <c r="H16" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I16" s="1">
         <v>4.6542852156779526</v>
@@ -991,7 +997,7 @@
         <v>2.4611205370017868</v>
       </c>
       <c r="H17" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I17" s="1">
         <v>4.2715165308090546</v>
@@ -1026,7 +1032,7 @@
         <v>2.0210962415748539</v>
       </c>
       <c r="H18" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I18" s="1">
         <v>4.4173485345120032</v>
@@ -1061,7 +1067,7 @@
         <v>2.0047812775642835</v>
       </c>
       <c r="H19" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I19" s="1">
         <v>4.4445241495861367</v>
@@ -1096,7 +1102,7 @@
         <v>1.8731439386793229</v>
       </c>
       <c r="H20" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I20" s="1">
         <v>5.4144292803451606</v>
@@ -1131,7 +1137,7 @@
         <v>1.6022140836252803</v>
       </c>
       <c r="H21" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I21" s="1">
         <v>5.9606971911011959</v>
@@ -1166,7 +1172,7 @@
         <v>2.0549475055926392</v>
       </c>
       <c r="H22" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I22" s="1">
         <v>5.9619596422091714</v>
@@ -1201,7 +1207,7 @@
         <v>2.1635018667518442</v>
       </c>
       <c r="H23" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I23" s="1">
         <v>5.9745516029577912</v>
@@ -1236,7 +1242,7 @@
         <v>1.5481777542137791</v>
       </c>
       <c r="H24" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I24" s="1">
         <v>5.487794975807283</v>
@@ -1271,7 +1277,7 @@
         <v>1.7170139729484681</v>
       </c>
       <c r="H25" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I25" s="1">
         <v>4.4593898112558827</v>
@@ -1306,7 +1312,7 @@
         <v>3.2453341512972078</v>
       </c>
       <c r="H26" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I26" s="1">
         <v>4.9051481990169776</v>
@@ -1341,7 +1347,7 @@
         <v>2.8314295624156745</v>
       </c>
       <c r="H27" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I27" s="1">
         <v>5.1625159043856375</v>
@@ -1376,7 +1382,7 @@
         <v>3.3796195901418034</v>
       </c>
       <c r="H28" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I28" s="1">
         <v>6.1772598553080611</v>
@@ -1411,7 +1417,7 @@
         <v>3.5066708574563585</v>
       </c>
       <c r="H29" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I29" s="1">
         <v>6.556186894042658</v>
@@ -1446,7 +1452,7 @@
         <v>3.8446688842753174</v>
       </c>
       <c r="H30" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I30" s="1">
         <v>7.0361815903898757</v>
@@ -1481,7 +1487,7 @@
         <v>2.7816817381932761</v>
       </c>
       <c r="H31" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I31" s="1">
         <v>6.9546991199255546</v>
@@ -1516,7 +1522,7 @@
         <v>3.5298957560305446</v>
       </c>
       <c r="H32" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I32" s="1">
         <v>6.2342441869814635</v>
@@ -1551,7 +1557,7 @@
         <v>4.5002924041878627</v>
       </c>
       <c r="H33" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I33" s="1">
         <v>5.6493469322113503</v>
@@ -1586,7 +1592,7 @@
         <v>3.246593360264499</v>
       </c>
       <c r="H34" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I34" s="1">
         <v>5.9353878829828908</v>
@@ -1621,7 +1627,7 @@
         <v>2.777505457025887</v>
       </c>
       <c r="H35" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I35" s="1">
         <v>6.214280874782121</v>
@@ -1656,7 +1662,7 @@
         <v>2.8656241961201157</v>
       </c>
       <c r="H36" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I36" s="1">
         <v>5.9263717750438145</v>
@@ -1691,7 +1697,7 @@
         <v>3.602411802477627</v>
       </c>
       <c r="H37" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I37" s="1">
         <v>5.8610806676661307</v>
@@ -1726,7 +1732,7 @@
         <v>3.4712443144576053</v>
       </c>
       <c r="H38" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I38" s="1">
         <v>6.2044998488071466</v>
@@ -1761,7 +1767,7 @@
         <v>3.5701152246303116</v>
       </c>
       <c r="H39" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I39" s="1">
         <v>5.8334041434884281</v>
@@ -1796,7 +1802,7 @@
         <v>2.254942260711331</v>
       </c>
       <c r="H40" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I40" s="1">
         <v>5.9712187990928589</v>
@@ -1831,7 +1837,7 @@
         <v>2.7144899914682092</v>
       </c>
       <c r="H41" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I41" s="1">
         <v>5.7931576191024865</v>
@@ -1866,7 +1872,7 @@
         <v>2.4421309148656056</v>
       </c>
       <c r="H42" s="1">
-        <v>9.9999999999999994E-12</v>
+        <v>0</v>
       </c>
       <c r="I42" s="1">
         <v>5.6530008904289835</v>
@@ -3311,6 +3317,2876 @@
       </c>
       <c r="K83" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>1975</v>
+      </c>
+      <c r="B84" s="1">
+        <v>5.8311674402625122E-2</v>
+      </c>
+      <c r="C84" s="1">
+        <v>0.29187722583635556</v>
+      </c>
+      <c r="D84" s="1">
+        <v>1.4547206492870602E-2</v>
+      </c>
+      <c r="E84" s="1">
+        <v>0.87322180962812435</v>
+      </c>
+      <c r="F84" s="1">
+        <v>0.85281657418091961</v>
+      </c>
+      <c r="G84" s="1">
+        <v>0.29780221585255545</v>
+      </c>
+      <c r="H84" s="1">
+        <v>0</v>
+      </c>
+      <c r="I84" s="1">
+        <v>0.21014334660824266</v>
+      </c>
+      <c r="J84" s="1">
+        <v>0.36957154380133234</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>1976</v>
+      </c>
+      <c r="B85" s="1">
+        <v>5.971407867671253E-2</v>
+      </c>
+      <c r="C85" s="1">
+        <v>0.27000023256856143</v>
+      </c>
+      <c r="D85" s="1">
+        <v>1.424961388890846E-2</v>
+      </c>
+      <c r="E85" s="1">
+        <v>0.87104442973774743</v>
+      </c>
+      <c r="F85" s="1">
+        <v>0.82004863600648392</v>
+      </c>
+      <c r="G85" s="1">
+        <v>0.32554461428488857</v>
+      </c>
+      <c r="H85" s="1">
+        <v>0</v>
+      </c>
+      <c r="I85" s="1">
+        <v>0.17136777705756526</v>
+      </c>
+      <c r="J85" s="1">
+        <v>0.33383308027367142</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>1977</v>
+      </c>
+      <c r="B86" s="1">
+        <v>6.18472651901118E-2</v>
+      </c>
+      <c r="C86" s="1">
+        <v>0.25479181025267117</v>
+      </c>
+      <c r="D86" s="1">
+        <v>1.4138017779323921E-2</v>
+      </c>
+      <c r="E86" s="1">
+        <v>0.87334656989073445</v>
+      </c>
+      <c r="F86" s="1">
+        <v>0.79689491756169117</v>
+      </c>
+      <c r="G86" s="1">
+        <v>0.31627580951960121</v>
+      </c>
+      <c r="H86" s="1">
+        <v>0</v>
+      </c>
+      <c r="I86" s="1">
+        <v>0.22083505828289887</v>
+      </c>
+      <c r="J86" s="1">
+        <v>0.31671702238106852</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>1978</v>
+      </c>
+      <c r="B87" s="1">
+        <v>7.0453570058374451E-2</v>
+      </c>
+      <c r="C87" s="1">
+        <v>0.26154395704080347</v>
+      </c>
+      <c r="D87" s="1">
+        <v>1.4937134834398668E-2</v>
+      </c>
+      <c r="E87" s="1">
+        <v>0.86496068774440094</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0.77312928370429079</v>
+      </c>
+      <c r="G87" s="1">
+        <v>0.32339277204319933</v>
+      </c>
+      <c r="H87" s="1">
+        <v>0</v>
+      </c>
+      <c r="I87" s="1">
+        <v>0.21184037016623886</v>
+      </c>
+      <c r="J87" s="1">
+        <v>0.265562429624422</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>1979</v>
+      </c>
+      <c r="B88" s="1">
+        <v>7.7214376853833797E-2</v>
+      </c>
+      <c r="C88" s="1">
+        <v>0.27182954471189458</v>
+      </c>
+      <c r="D88" s="1">
+        <v>1.8399164988687149E-2</v>
+      </c>
+      <c r="E88" s="1">
+        <v>0.85164648196923221</v>
+      </c>
+      <c r="F88" s="1">
+        <v>0.76700035147921031</v>
+      </c>
+      <c r="G88" s="1">
+        <v>0.24454412914741749</v>
+      </c>
+      <c r="H88" s="1">
+        <v>0</v>
+      </c>
+      <c r="I88" s="1">
+        <v>0.22154753504298669</v>
+      </c>
+      <c r="J88" s="1">
+        <v>0.24718662783418749</v>
+      </c>
+      <c r="K88" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>1980</v>
+      </c>
+      <c r="B89" s="1">
+        <v>8.0263776539113874E-2</v>
+      </c>
+      <c r="C89" s="1">
+        <v>0.28278186759612689</v>
+      </c>
+      <c r="D89" s="1">
+        <v>1.5675392437735122E-2</v>
+      </c>
+      <c r="E89" s="1">
+        <v>0.83770367426750303</v>
+      </c>
+      <c r="F89" s="1">
+        <v>0.75326436769519722</v>
+      </c>
+      <c r="G89" s="1">
+        <v>0.35876794949276103</v>
+      </c>
+      <c r="H89" s="1">
+        <v>0</v>
+      </c>
+      <c r="I89" s="1">
+        <v>0.22858775239505263</v>
+      </c>
+      <c r="J89" s="1">
+        <v>0.23483481407781481</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>1981</v>
+      </c>
+      <c r="B90" s="1">
+        <v>8.1895472225121183E-2</v>
+      </c>
+      <c r="C90" s="1">
+        <v>0.2571728251483556</v>
+      </c>
+      <c r="D90" s="1">
+        <v>1.2999820449641149E-2</v>
+      </c>
+      <c r="E90" s="1">
+        <v>0.81596041662722507</v>
+      </c>
+      <c r="F90" s="1">
+        <v>0.75692532956738434</v>
+      </c>
+      <c r="G90" s="1">
+        <v>0.34133186682709471</v>
+      </c>
+      <c r="H90" s="1">
+        <v>0</v>
+      </c>
+      <c r="I90" s="1">
+        <v>0.2952981013123227</v>
+      </c>
+      <c r="J90" s="1">
+        <v>0.19678893184570076</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>1982</v>
+      </c>
+      <c r="B91" s="1">
+        <v>8.3315721911614959E-2</v>
+      </c>
+      <c r="C91" s="1">
+        <v>0.25213662517000351</v>
+      </c>
+      <c r="D91" s="1">
+        <v>1.5304954549127397E-2</v>
+      </c>
+      <c r="E91" s="1">
+        <v>0.83414439005336405</v>
+      </c>
+      <c r="F91" s="1">
+        <v>0.74097426656966636</v>
+      </c>
+      <c r="G91" s="1">
+        <v>0.35067881892554842</v>
+      </c>
+      <c r="H91" s="1">
+        <v>0</v>
+      </c>
+      <c r="I91" s="1">
+        <v>0.21152603434538431</v>
+      </c>
+      <c r="J91" s="1">
+        <v>0.18370591448026152</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>1983</v>
+      </c>
+      <c r="B92" s="1">
+        <v>8.6219175981053192E-2</v>
+      </c>
+      <c r="C92" s="1">
+        <v>0.25315431718821618</v>
+      </c>
+      <c r="D92" s="1">
+        <v>1.571267381136374E-2</v>
+      </c>
+      <c r="E92" s="1">
+        <v>0.84180530901786521</v>
+      </c>
+      <c r="F92" s="1">
+        <v>0.72320657267242594</v>
+      </c>
+      <c r="G92" s="1">
+        <v>0.25850095958645619</v>
+      </c>
+      <c r="H92" s="1">
+        <v>0</v>
+      </c>
+      <c r="I92" s="1">
+        <v>0.2261678094629396</v>
+      </c>
+      <c r="J92" s="1">
+        <v>0.1733637877523253</v>
+      </c>
+      <c r="K92" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>1984</v>
+      </c>
+      <c r="B93" s="1">
+        <v>9.1791509354549522E-2</v>
+      </c>
+      <c r="C93" s="1">
+        <v>0.25342204442397287</v>
+      </c>
+      <c r="D93" s="1">
+        <v>1.4707942142992715E-2</v>
+      </c>
+      <c r="E93" s="1">
+        <v>0.84651210828854118</v>
+      </c>
+      <c r="F93" s="1">
+        <v>0.71551174841672205</v>
+      </c>
+      <c r="G93" s="1">
+        <v>0.24217216171504583</v>
+      </c>
+      <c r="H93" s="1">
+        <v>0</v>
+      </c>
+      <c r="I93" s="1">
+        <v>0.27882219737823266</v>
+      </c>
+      <c r="J93" s="1">
+        <v>0.16929784521414953</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>1985</v>
+      </c>
+      <c r="B94" s="1">
+        <v>9.3636578827677605E-2</v>
+      </c>
+      <c r="C94" s="1">
+        <v>0.2531552447976459</v>
+      </c>
+      <c r="D94" s="1">
+        <v>1.3829370490274351E-2</v>
+      </c>
+      <c r="E94" s="1">
+        <v>0.84988263762410288</v>
+      </c>
+      <c r="F94" s="1">
+        <v>0.70578104826317112</v>
+      </c>
+      <c r="G94" s="1">
+        <v>0.25094233562044166</v>
+      </c>
+      <c r="H94" s="1">
+        <v>0</v>
+      </c>
+      <c r="I94" s="1">
+        <v>0.2787057552943612</v>
+      </c>
+      <c r="J94" s="1">
+        <v>0.16231725354551427</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>1986</v>
+      </c>
+      <c r="B95" s="1">
+        <v>9.6393870463496636E-2</v>
+      </c>
+      <c r="C95" s="1">
+        <v>0.27032590795547684</v>
+      </c>
+      <c r="D95" s="1">
+        <v>1.1523524878980885E-2</v>
+      </c>
+      <c r="E95" s="1">
+        <v>0.84661751253841411</v>
+      </c>
+      <c r="F95" s="1">
+        <v>0.70133927427684217</v>
+      </c>
+      <c r="G95" s="1">
+        <v>0.24974560718266123</v>
+      </c>
+      <c r="H95" s="1">
+        <v>0</v>
+      </c>
+      <c r="I95" s="1">
+        <v>0.28758931336848126</v>
+      </c>
+      <c r="J95" s="1">
+        <v>0.1583493629874809</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>1987</v>
+      </c>
+      <c r="B96" s="1">
+        <v>9.4816860863135718E-2</v>
+      </c>
+      <c r="C96" s="1">
+        <v>0.27651421622139266</v>
+      </c>
+      <c r="D96" s="1">
+        <v>1.0434491857322576E-2</v>
+      </c>
+      <c r="E96" s="1">
+        <v>0.85348025412111361</v>
+      </c>
+      <c r="F96" s="1">
+        <v>0.69628757121738627</v>
+      </c>
+      <c r="G96" s="1">
+        <v>0.25683155919910494</v>
+      </c>
+      <c r="H96" s="1">
+        <v>0</v>
+      </c>
+      <c r="I96" s="1">
+        <v>0.26453146315425313</v>
+      </c>
+      <c r="J96" s="1">
+        <v>0.16392701993982073</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>1988</v>
+      </c>
+      <c r="B97" s="1">
+        <v>9.3289306426658808E-2</v>
+      </c>
+      <c r="C97" s="1">
+        <v>0.26808608010386253</v>
+      </c>
+      <c r="D97" s="1">
+        <v>1.0021207158186565E-2</v>
+      </c>
+      <c r="E97" s="1">
+        <v>0.8538780394020018</v>
+      </c>
+      <c r="F97" s="1">
+        <v>0.69161435338754695</v>
+      </c>
+      <c r="G97" s="1">
+        <v>0.18457695207216826</v>
+      </c>
+      <c r="H97" s="1">
+        <v>0</v>
+      </c>
+      <c r="I97" s="1">
+        <v>0.34783037917243154</v>
+      </c>
+      <c r="J97" s="1">
+        <v>0.16660573413819771</v>
+      </c>
+      <c r="K97" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>1989</v>
+      </c>
+      <c r="B98" s="1">
+        <v>8.9857936655611315E-2</v>
+      </c>
+      <c r="C98" s="1">
+        <v>0.2553369995877085</v>
+      </c>
+      <c r="D98" s="1">
+        <v>9.8707010635727122E-3</v>
+      </c>
+      <c r="E98" s="1">
+        <v>0.84934339919802204</v>
+      </c>
+      <c r="F98" s="1">
+        <v>0.6840817855668464</v>
+      </c>
+      <c r="G98" s="1">
+        <v>0.18654166730510111</v>
+      </c>
+      <c r="H98" s="1">
+        <v>0</v>
+      </c>
+      <c r="I98" s="1">
+        <v>0.43291281689111605</v>
+      </c>
+      <c r="J98" s="1">
+        <v>0.16956913328086914</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>1990</v>
+      </c>
+      <c r="B99" s="1">
+        <v>9.8395305455026033E-2</v>
+      </c>
+      <c r="C99" s="1">
+        <v>0.23666960618166608</v>
+      </c>
+      <c r="D99" s="1">
+        <v>9.5722144744084681E-3</v>
+      </c>
+      <c r="E99" s="1">
+        <v>0.8477084800906135</v>
+      </c>
+      <c r="F99" s="1">
+        <v>0.67133255561989702</v>
+      </c>
+      <c r="G99" s="1">
+        <v>0.18052283065563499</v>
+      </c>
+      <c r="H99" s="1">
+        <v>0</v>
+      </c>
+      <c r="I99" s="1">
+        <v>0.39388462249152678</v>
+      </c>
+      <c r="J99" s="1">
+        <v>0.15639122736135017</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>1991</v>
+      </c>
+      <c r="B100" s="1">
+        <v>0.1000381806929307</v>
+      </c>
+      <c r="C100" s="1">
+        <v>0.23155597256421806</v>
+      </c>
+      <c r="D100" s="1">
+        <v>8.9977086846712451E-3</v>
+      </c>
+      <c r="E100" s="1">
+        <v>0.84371488723028576</v>
+      </c>
+      <c r="F100" s="1">
+        <v>0.66188551586894728</v>
+      </c>
+      <c r="G100" s="1">
+        <v>0.16853523050701466</v>
+      </c>
+      <c r="H100" s="1">
+        <v>0</v>
+      </c>
+      <c r="I100" s="1">
+        <v>0.41723431722222276</v>
+      </c>
+      <c r="J100" s="1">
+        <v>0.14709334179815414</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>1992</v>
+      </c>
+      <c r="B101" s="1">
+        <v>0.10074436795181826</v>
+      </c>
+      <c r="C101" s="1">
+        <v>0.23206628927636958</v>
+      </c>
+      <c r="D101" s="1">
+        <v>9.0710019449306255E-3</v>
+      </c>
+      <c r="E101" s="1">
+        <v>0.84710551867327955</v>
+      </c>
+      <c r="F101" s="1">
+        <v>0.65886072926732198</v>
+      </c>
+      <c r="G101" s="1">
+        <v>0.17643775487070562</v>
+      </c>
+      <c r="H101" s="1">
+        <v>0</v>
+      </c>
+      <c r="I101" s="1">
+        <v>0.43200894515755178</v>
+      </c>
+      <c r="J101" s="1">
+        <v>0.14918221361924303</v>
+      </c>
+      <c r="K101" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>1993</v>
+      </c>
+      <c r="B102" s="1">
+        <v>0.10557850169675322</v>
+      </c>
+      <c r="C102" s="1">
+        <v>0.24537563420215591</v>
+      </c>
+      <c r="D102" s="1">
+        <v>9.3486013432638841E-3</v>
+      </c>
+      <c r="E102" s="1">
+        <v>0.85758148528511335</v>
+      </c>
+      <c r="F102" s="1">
+        <v>0.66853653820495784</v>
+      </c>
+      <c r="G102" s="1">
+        <v>0.18182203312524259</v>
+      </c>
+      <c r="H102" s="1">
+        <v>0</v>
+      </c>
+      <c r="I102" s="1">
+        <v>0.49712289567911089</v>
+      </c>
+      <c r="J102" s="1">
+        <v>0.16080563655845276</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>1994</v>
+      </c>
+      <c r="B103" s="1">
+        <v>0.107465715544985</v>
+      </c>
+      <c r="C103" s="1">
+        <v>0.25028867783110959</v>
+      </c>
+      <c r="D103" s="1">
+        <v>9.6086016700896067E-3</v>
+      </c>
+      <c r="E103" s="1">
+        <v>0.86845122185512957</v>
+      </c>
+      <c r="F103" s="1">
+        <v>0.67591110569508317</v>
+      </c>
+      <c r="G103" s="1">
+        <v>0.14503746132999917</v>
+      </c>
+      <c r="H103" s="1">
+        <v>0</v>
+      </c>
+      <c r="I103" s="1">
+        <v>0.51316144631974958</v>
+      </c>
+      <c r="J103" s="1">
+        <v>0.16208108688714953</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>1995</v>
+      </c>
+      <c r="B104" s="1">
+        <v>9.8302175997363461E-2</v>
+      </c>
+      <c r="C104" s="1">
+        <v>0.24534112497791302</v>
+      </c>
+      <c r="D104" s="1">
+        <v>1.0274368692170913E-2</v>
+      </c>
+      <c r="E104" s="1">
+        <v>0.87867437934240211</v>
+      </c>
+      <c r="F104" s="1">
+        <v>0.66960543771165781</v>
+      </c>
+      <c r="G104" s="1">
+        <v>0.19404338644199262</v>
+      </c>
+      <c r="H104" s="1">
+        <v>0</v>
+      </c>
+      <c r="I104" s="1">
+        <v>0.52061302981285451</v>
+      </c>
+      <c r="J104" s="1">
+        <v>0.17741967819921628</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>1996</v>
+      </c>
+      <c r="B105" s="1">
+        <v>9.2722420470381872E-2</v>
+      </c>
+      <c r="C105" s="1">
+        <v>0.24208907806421121</v>
+      </c>
+      <c r="D105" s="1">
+        <v>1.10903716957821E-2</v>
+      </c>
+      <c r="E105" s="1">
+        <v>0.88656860526869363</v>
+      </c>
+      <c r="F105" s="1">
+        <v>0.68125836142511909</v>
+      </c>
+      <c r="G105" s="1">
+        <v>0.21946261450986604</v>
+      </c>
+      <c r="H105" s="1">
+        <v>0</v>
+      </c>
+      <c r="I105" s="1">
+        <v>0.53135540341675591</v>
+      </c>
+      <c r="J105" s="1">
+        <v>0.17544429057754568</v>
+      </c>
+      <c r="K105" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>1997</v>
+      </c>
+      <c r="B106" s="1">
+        <v>9.4489476851291179E-2</v>
+      </c>
+      <c r="C106" s="1">
+        <v>0.23779292490114481</v>
+      </c>
+      <c r="D106" s="1">
+        <v>1.080837656559961E-2</v>
+      </c>
+      <c r="E106" s="1">
+        <v>0.89272190927539075</v>
+      </c>
+      <c r="F106" s="1">
+        <v>0.68730007852795338</v>
+      </c>
+      <c r="G106" s="1">
+        <v>0.17169500500495946</v>
+      </c>
+      <c r="H106" s="1">
+        <v>0</v>
+      </c>
+      <c r="I106" s="1">
+        <v>0.51483524492522503</v>
+      </c>
+      <c r="J106" s="1">
+        <v>0.17362031808082345</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>1998</v>
+      </c>
+      <c r="B107" s="1">
+        <v>9.029863335711158E-2</v>
+      </c>
+      <c r="C107" s="1">
+        <v>0.23557287552225917</v>
+      </c>
+      <c r="D107" s="1">
+        <v>1.2173850758549662E-2</v>
+      </c>
+      <c r="E107" s="1">
+        <v>0.89670060283498942</v>
+      </c>
+      <c r="F107" s="1">
+        <v>0.68250706327797617</v>
+      </c>
+      <c r="G107" s="1">
+        <v>0.18574948046654599</v>
+      </c>
+      <c r="H107" s="1">
+        <v>0</v>
+      </c>
+      <c r="I107" s="1">
+        <v>0.45238561352324258</v>
+      </c>
+      <c r="J107" s="1">
+        <v>0.19628608174000883</v>
+      </c>
+      <c r="K107" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B108" s="1">
+        <v>9.0967290913413656E-2</v>
+      </c>
+      <c r="C108" s="1">
+        <v>0.24020660857956433</v>
+      </c>
+      <c r="D108" s="1">
+        <v>1.2327305906583139E-2</v>
+      </c>
+      <c r="E108" s="1">
+        <v>0.89616794881217543</v>
+      </c>
+      <c r="F108" s="1">
+        <v>0.66532385857655785</v>
+      </c>
+      <c r="G108" s="1">
+        <v>0.25138805320739871</v>
+      </c>
+      <c r="H108" s="1">
+        <v>0</v>
+      </c>
+      <c r="I108" s="1">
+        <v>0.47886403137853406</v>
+      </c>
+      <c r="J108" s="1">
+        <v>0.20921121576979412</v>
+      </c>
+      <c r="K108" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B109" s="1">
+        <v>8.9974864308906596E-2</v>
+      </c>
+      <c r="C109" s="1">
+        <v>0.24490805676197291</v>
+      </c>
+      <c r="D109" s="1">
+        <v>1.326187706664925E-2</v>
+      </c>
+      <c r="E109" s="1">
+        <v>0.89566110948802302</v>
+      </c>
+      <c r="F109" s="1">
+        <v>0.65035938668803606</v>
+      </c>
+      <c r="G109" s="1">
+        <v>0.20945537809937767</v>
+      </c>
+      <c r="H109" s="1">
+        <v>0</v>
+      </c>
+      <c r="I109" s="1">
+        <v>0.48696029396764856</v>
+      </c>
+      <c r="J109" s="1">
+        <v>0.20743882572761871</v>
+      </c>
+      <c r="K109" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B110" s="1">
+        <v>9.2794549926860023E-2</v>
+      </c>
+      <c r="C110" s="1">
+        <v>0.23642772835206857</v>
+      </c>
+      <c r="D110" s="1">
+        <v>1.0492793105791289E-2</v>
+      </c>
+      <c r="E110" s="1">
+        <v>0.90319901606628594</v>
+      </c>
+      <c r="F110" s="1">
+        <v>0.63667967125623537</v>
+      </c>
+      <c r="G110" s="1">
+        <v>0.24148828901412664</v>
+      </c>
+      <c r="H110" s="1">
+        <v>0</v>
+      </c>
+      <c r="I110" s="1">
+        <v>0.533368708843593</v>
+      </c>
+      <c r="J110" s="1">
+        <v>0.19914514157312094</v>
+      </c>
+      <c r="K110" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B111" s="1">
+        <v>9.658763226941304E-2</v>
+      </c>
+      <c r="C111" s="1">
+        <v>0.24023534615416015</v>
+      </c>
+      <c r="D111" s="1">
+        <v>1.7090884165751039E-2</v>
+      </c>
+      <c r="E111" s="1">
+        <v>0.90956258752458963</v>
+      </c>
+      <c r="F111" s="1">
+        <v>0.63044422246348897</v>
+      </c>
+      <c r="G111" s="1">
+        <v>0.24984606416696414</v>
+      </c>
+      <c r="H111" s="1">
+        <v>0</v>
+      </c>
+      <c r="I111" s="1">
+        <v>0.55245145361873527</v>
+      </c>
+      <c r="J111" s="1">
+        <v>0.22239324108985403</v>
+      </c>
+      <c r="K111" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B112" s="1">
+        <v>9.1884326787151319E-2</v>
+      </c>
+      <c r="C112" s="1">
+        <v>0.23882600791407155</v>
+      </c>
+      <c r="D112" s="1">
+        <v>1.208056830472121E-2</v>
+      </c>
+      <c r="E112" s="1">
+        <v>0.91077289063158806</v>
+      </c>
+      <c r="F112" s="1">
+        <v>0.62473478225248402</v>
+      </c>
+      <c r="G112" s="1">
+        <v>0.25397048623498775</v>
+      </c>
+      <c r="H112" s="1">
+        <v>0</v>
+      </c>
+      <c r="I112" s="1">
+        <v>0.56090067974162106</v>
+      </c>
+      <c r="J112" s="1">
+        <v>0.22620383401521912</v>
+      </c>
+      <c r="K112" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B113" s="1">
+        <v>9.3332435023556412E-2</v>
+      </c>
+      <c r="C113" s="1">
+        <v>0.25173727305014504</v>
+      </c>
+      <c r="D113" s="1">
+        <v>1.342165534989085E-2</v>
+      </c>
+      <c r="E113" s="1">
+        <v>0.91509850681692095</v>
+      </c>
+      <c r="F113" s="1">
+        <v>0.62048631246058916</v>
+      </c>
+      <c r="G113" s="1">
+        <v>0.19945300717651526</v>
+      </c>
+      <c r="H113" s="1">
+        <v>0</v>
+      </c>
+      <c r="I113" s="1">
+        <v>0.56110356613951218</v>
+      </c>
+      <c r="J113" s="1">
+        <v>0.21975997871735653</v>
+      </c>
+      <c r="K113" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B114" s="1">
+        <v>9.3660811776561825E-2</v>
+      </c>
+      <c r="C114" s="1">
+        <v>0.24482230125474952</v>
+      </c>
+      <c r="D114" s="1">
+        <v>1.3682873079808353E-2</v>
+      </c>
+      <c r="E114" s="1">
+        <v>0.92479354055913554</v>
+      </c>
+      <c r="F114" s="1">
+        <v>0.61546605399894727</v>
+      </c>
+      <c r="G114" s="1">
+        <v>0.22436930747983636</v>
+      </c>
+      <c r="H114" s="1">
+        <v>0</v>
+      </c>
+      <c r="I114" s="1">
+        <v>0.52642585399114217</v>
+      </c>
+      <c r="J114" s="1">
+        <v>0.22027257548646853</v>
+      </c>
+      <c r="K114" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B115" s="1">
+        <v>9.1039191066484559E-2</v>
+      </c>
+      <c r="C115" s="1">
+        <v>0.2626368931948676</v>
+      </c>
+      <c r="D115" s="1">
+        <v>1.5164169482674957E-2</v>
+      </c>
+      <c r="E115" s="1">
+        <v>0.9254080626575022</v>
+      </c>
+      <c r="F115" s="1">
+        <v>0.61730512078655908</v>
+      </c>
+      <c r="G115" s="1">
+        <v>0.28381285938676365</v>
+      </c>
+      <c r="H115" s="1">
+        <v>0</v>
+      </c>
+      <c r="I115" s="1">
+        <v>0.5166801786080415</v>
+      </c>
+      <c r="J115" s="1">
+        <v>0.2227029484165704</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B116" s="1">
+        <v>8.9403864582664666E-2</v>
+      </c>
+      <c r="C116" s="1">
+        <v>0.26932675007624574</v>
+      </c>
+      <c r="D116" s="1">
+        <v>1.1332044928818313E-2</v>
+      </c>
+      <c r="E116" s="1">
+        <v>0.92402936254713075</v>
+      </c>
+      <c r="F116" s="1">
+        <v>0.61594670901998294</v>
+      </c>
+      <c r="G116" s="1">
+        <v>0.21375693143948377</v>
+      </c>
+      <c r="H116" s="1">
+        <v>0</v>
+      </c>
+      <c r="I116" s="1">
+        <v>0.52437249165145905</v>
+      </c>
+      <c r="J116" s="1">
+        <v>0.21538913865752329</v>
+      </c>
+      <c r="K116" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B117" s="1">
+        <v>8.9327070477088238E-2</v>
+      </c>
+      <c r="C117" s="1">
+        <v>0.27119257937870095</v>
+      </c>
+      <c r="D117" s="1">
+        <v>1.6415085726836681E-2</v>
+      </c>
+      <c r="E117" s="1">
+        <v>0.92109391089796799</v>
+      </c>
+      <c r="F117" s="1">
+        <v>0.61493059512217718</v>
+      </c>
+      <c r="G117" s="1">
+        <v>0.17218632043424384</v>
+      </c>
+      <c r="H117" s="1">
+        <v>0</v>
+      </c>
+      <c r="I117" s="1">
+        <v>0.55951779678104807</v>
+      </c>
+      <c r="J117" s="1">
+        <v>0.19620144580966553</v>
+      </c>
+      <c r="K117" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B118" s="1">
+        <v>9.1190594489666377E-2</v>
+      </c>
+      <c r="C118" s="1">
+        <v>0.27588288163998986</v>
+      </c>
+      <c r="D118" s="1">
+        <v>1.5493512006842486E-2</v>
+      </c>
+      <c r="E118" s="1">
+        <v>0.9157380833101636</v>
+      </c>
+      <c r="F118" s="1">
+        <v>0.61078443971005147</v>
+      </c>
+      <c r="G118" s="1">
+        <v>0.17319857137801492</v>
+      </c>
+      <c r="H118" s="1">
+        <v>0</v>
+      </c>
+      <c r="I118" s="1">
+        <v>0.5560345174435356</v>
+      </c>
+      <c r="J118" s="1">
+        <v>0.1927765142219969</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B119" s="1">
+        <v>9.0708695885717242E-2</v>
+      </c>
+      <c r="C119" s="1">
+        <v>0.27929296732872094</v>
+      </c>
+      <c r="D119" s="1">
+        <v>1.0630465316611413E-2</v>
+      </c>
+      <c r="E119" s="1">
+        <v>0.9097373772756151</v>
+      </c>
+      <c r="F119" s="1">
+        <v>0.63784884457199731</v>
+      </c>
+      <c r="G119" s="1">
+        <v>0.20364973458642957</v>
+      </c>
+      <c r="H119" s="1">
+        <v>0</v>
+      </c>
+      <c r="I119" s="1">
+        <v>0.5753272735677567</v>
+      </c>
+      <c r="J119" s="1">
+        <v>0.23851347074854976</v>
+      </c>
+      <c r="K119" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B120" s="1">
+        <v>8.8534378988803786E-2</v>
+      </c>
+      <c r="C120" s="1">
+        <v>0.27966275393867507</v>
+      </c>
+      <c r="D120" s="1">
+        <v>1.3349932424501065E-2</v>
+      </c>
+      <c r="E120" s="1">
+        <v>0.90774627534257657</v>
+      </c>
+      <c r="F120" s="1">
+        <v>0.63679863857109131</v>
+      </c>
+      <c r="G120" s="1">
+        <v>0.20626965866062785</v>
+      </c>
+      <c r="H120" s="1">
+        <v>0</v>
+      </c>
+      <c r="I120" s="1">
+        <v>0.59161555187023507</v>
+      </c>
+      <c r="J120" s="1">
+        <v>0.24468632982536251</v>
+      </c>
+      <c r="K120" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B121" s="1">
+        <v>9.1295852046312354E-2</v>
+      </c>
+      <c r="C121" s="1">
+        <v>0.2841243115784281</v>
+      </c>
+      <c r="D121" s="1">
+        <v>1.4881818200444945E-2</v>
+      </c>
+      <c r="E121" s="1">
+        <v>0.90730858802019843</v>
+      </c>
+      <c r="F121" s="1">
+        <v>0.63966657332096377</v>
+      </c>
+      <c r="G121" s="1">
+        <v>0.20945406029982483</v>
+      </c>
+      <c r="H121" s="1">
+        <v>0</v>
+      </c>
+      <c r="I121" s="1">
+        <v>0.57191527901703665</v>
+      </c>
+      <c r="J121" s="1">
+        <v>0.2379341929626011</v>
+      </c>
+      <c r="K121" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B122" s="1">
+        <v>9.4484012967354633E-2</v>
+      </c>
+      <c r="C122" s="1">
+        <v>0.29182081206420946</v>
+      </c>
+      <c r="D122" s="1">
+        <v>1.2472458489215195E-2</v>
+      </c>
+      <c r="E122" s="1">
+        <v>0.91049532828042146</v>
+      </c>
+      <c r="F122" s="1">
+        <v>0.63935688979176808</v>
+      </c>
+      <c r="G122" s="1">
+        <v>0.15661404612325966</v>
+      </c>
+      <c r="H122" s="1">
+        <v>0</v>
+      </c>
+      <c r="I122" s="1">
+        <v>0.57739744371982527</v>
+      </c>
+      <c r="J122" s="1">
+        <v>0.25978499987068171</v>
+      </c>
+      <c r="K122" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B123" s="1">
+        <v>9.5143781930063662E-2</v>
+      </c>
+      <c r="C123" s="1">
+        <v>0.29624090197082348</v>
+      </c>
+      <c r="D123" s="1">
+        <v>1.2502663159495761E-2</v>
+      </c>
+      <c r="E123" s="1">
+        <v>0.91193607494752249</v>
+      </c>
+      <c r="F123" s="1">
+        <v>0.63660466709078989</v>
+      </c>
+      <c r="G123" s="1">
+        <v>0.16796710929080574</v>
+      </c>
+      <c r="H123" s="1">
+        <v>0</v>
+      </c>
+      <c r="I123" s="1">
+        <v>0.57447185602493955</v>
+      </c>
+      <c r="J123" s="1">
+        <v>0.25799909578870089</v>
+      </c>
+      <c r="K123" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B124" s="1">
+        <v>9.6058117583686264E-2</v>
+      </c>
+      <c r="C124" s="1">
+        <v>0.29712056608534804</v>
+      </c>
+      <c r="D124" s="1">
+        <v>1.3225174482661105E-2</v>
+      </c>
+      <c r="E124" s="1">
+        <v>0.91158945286442139</v>
+      </c>
+      <c r="F124" s="1">
+        <v>0.63403477483457815</v>
+      </c>
+      <c r="G124" s="1">
+        <v>0.17948846881633815</v>
+      </c>
+      <c r="H124" s="1">
+        <v>0</v>
+      </c>
+      <c r="I124" s="1">
+        <v>0.5706508792152668</v>
+      </c>
+      <c r="J124" s="1">
+        <v>0.26043486416220013</v>
+      </c>
+      <c r="K124" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <v>1975</v>
+      </c>
+      <c r="B125" s="1">
+        <v>0.94168832559737492</v>
+      </c>
+      <c r="C125" s="1">
+        <v>0.70812277416364444</v>
+      </c>
+      <c r="D125" s="1">
+        <v>0.98545279350712944</v>
+      </c>
+      <c r="E125" s="1">
+        <v>0.1267781903718756</v>
+      </c>
+      <c r="F125" s="1">
+        <v>0.14718342581908037</v>
+      </c>
+      <c r="G125" s="1">
+        <v>0.70219778414744449</v>
+      </c>
+      <c r="H125" s="1">
+        <v>1</v>
+      </c>
+      <c r="I125" s="1">
+        <v>0.78985665339175737</v>
+      </c>
+      <c r="J125" s="1">
+        <v>0.63042845619866772</v>
+      </c>
+      <c r="K125" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
+        <v>1976</v>
+      </c>
+      <c r="B126" s="1">
+        <v>0.94028592132328737</v>
+      </c>
+      <c r="C126" s="1">
+        <v>0.72999976743143857</v>
+      </c>
+      <c r="D126" s="1">
+        <v>0.98575038611109145</v>
+      </c>
+      <c r="E126" s="1">
+        <v>0.12895557026225249</v>
+      </c>
+      <c r="F126" s="1">
+        <v>0.17995136399351605</v>
+      </c>
+      <c r="G126" s="1">
+        <v>0.67445538571511132</v>
+      </c>
+      <c r="H126" s="1">
+        <v>1</v>
+      </c>
+      <c r="I126" s="1">
+        <v>0.82863222294243466</v>
+      </c>
+      <c r="J126" s="1">
+        <v>0.66616691972632847</v>
+      </c>
+      <c r="K126" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
+        <v>1977</v>
+      </c>
+      <c r="B127" s="1">
+        <v>0.93815273480988826</v>
+      </c>
+      <c r="C127" s="1">
+        <v>0.74520818974732894</v>
+      </c>
+      <c r="D127" s="1">
+        <v>0.98586198222067623</v>
+      </c>
+      <c r="E127" s="1">
+        <v>0.12665343010926552</v>
+      </c>
+      <c r="F127" s="1">
+        <v>0.20310508243830888</v>
+      </c>
+      <c r="G127" s="1">
+        <v>0.68372419048039867</v>
+      </c>
+      <c r="H127" s="1">
+        <v>1</v>
+      </c>
+      <c r="I127" s="1">
+        <v>0.77916494171710116</v>
+      </c>
+      <c r="J127" s="1">
+        <v>0.68328297761893153</v>
+      </c>
+      <c r="K127" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
+        <v>1978</v>
+      </c>
+      <c r="B128" s="1">
+        <v>0.92954642994162551</v>
+      </c>
+      <c r="C128" s="1">
+        <v>0.73845604295919653</v>
+      </c>
+      <c r="D128" s="1">
+        <v>0.98506286516560126</v>
+      </c>
+      <c r="E128" s="1">
+        <v>0.13503931225559904</v>
+      </c>
+      <c r="F128" s="1">
+        <v>0.22687071629570912</v>
+      </c>
+      <c r="G128" s="1">
+        <v>0.67660722795680062</v>
+      </c>
+      <c r="H128" s="1">
+        <v>1</v>
+      </c>
+      <c r="I128" s="1">
+        <v>0.7881596298337612</v>
+      </c>
+      <c r="J128" s="1">
+        <v>0.734437570375578</v>
+      </c>
+      <c r="K128" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <v>1979</v>
+      </c>
+      <c r="B129" s="1">
+        <v>0.92278562314616619</v>
+      </c>
+      <c r="C129" s="1">
+        <v>0.72817045528810542</v>
+      </c>
+      <c r="D129" s="1">
+        <v>0.98160083501131279</v>
+      </c>
+      <c r="E129" s="1">
+        <v>0.14835351803076788</v>
+      </c>
+      <c r="F129" s="1">
+        <v>0.23299964852078975</v>
+      </c>
+      <c r="G129" s="1">
+        <v>0.75545587085258248</v>
+      </c>
+      <c r="H129" s="1">
+        <v>1</v>
+      </c>
+      <c r="I129" s="1">
+        <v>0.77845246495701326</v>
+      </c>
+      <c r="J129" s="1">
+        <v>0.75281337216581257</v>
+      </c>
+      <c r="K129" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
+        <v>1980</v>
+      </c>
+      <c r="B130" s="1">
+        <v>0.91973622346088613</v>
+      </c>
+      <c r="C130" s="1">
+        <v>0.71721813240387322</v>
+      </c>
+      <c r="D130" s="1">
+        <v>0.98432460756226492</v>
+      </c>
+      <c r="E130" s="1">
+        <v>0.16229632573249689</v>
+      </c>
+      <c r="F130" s="1">
+        <v>0.24673563230480278</v>
+      </c>
+      <c r="G130" s="1">
+        <v>0.64123205050723897</v>
+      </c>
+      <c r="H130" s="1">
+        <v>1</v>
+      </c>
+      <c r="I130" s="1">
+        <v>0.77141224760494742</v>
+      </c>
+      <c r="J130" s="1">
+        <v>0.76516518592218519</v>
+      </c>
+      <c r="K130" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
+        <v>1981</v>
+      </c>
+      <c r="B131" s="1">
+        <v>0.91810452777487883</v>
+      </c>
+      <c r="C131" s="1">
+        <v>0.7428271748516444</v>
+      </c>
+      <c r="D131" s="1">
+        <v>0.98700017955035879</v>
+      </c>
+      <c r="E131" s="1">
+        <v>0.18403958337277496</v>
+      </c>
+      <c r="F131" s="1">
+        <v>0.24307467043261563</v>
+      </c>
+      <c r="G131" s="1">
+        <v>0.65866813317290529</v>
+      </c>
+      <c r="H131" s="1">
+        <v>1</v>
+      </c>
+      <c r="I131" s="1">
+        <v>0.70470189868767719</v>
+      </c>
+      <c r="J131" s="1">
+        <v>0.80321106815429921</v>
+      </c>
+      <c r="K131" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
+        <v>1982</v>
+      </c>
+      <c r="B132" s="1">
+        <v>0.91668427808838504</v>
+      </c>
+      <c r="C132" s="1">
+        <v>0.74786337482999654</v>
+      </c>
+      <c r="D132" s="1">
+        <v>0.98469504545087261</v>
+      </c>
+      <c r="E132" s="1">
+        <v>0.16585560994663587</v>
+      </c>
+      <c r="F132" s="1">
+        <v>0.25902573343033364</v>
+      </c>
+      <c r="G132" s="1">
+        <v>0.64932118107445169</v>
+      </c>
+      <c r="H132" s="1">
+        <v>1</v>
+      </c>
+      <c r="I132" s="1">
+        <v>0.7884739656546158</v>
+      </c>
+      <c r="J132" s="1">
+        <v>0.81629408551973848</v>
+      </c>
+      <c r="K132" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <v>1983</v>
+      </c>
+      <c r="B133" s="1">
+        <v>0.91378082401894689</v>
+      </c>
+      <c r="C133" s="1">
+        <v>0.74684568281178387</v>
+      </c>
+      <c r="D133" s="1">
+        <v>0.98428732618863624</v>
+      </c>
+      <c r="E133" s="1">
+        <v>0.15819469098213479</v>
+      </c>
+      <c r="F133" s="1">
+        <v>0.276793427327574</v>
+      </c>
+      <c r="G133" s="1">
+        <v>0.74149904041354375</v>
+      </c>
+      <c r="H133" s="1">
+        <v>1</v>
+      </c>
+      <c r="I133" s="1">
+        <v>0.77383219053706043</v>
+      </c>
+      <c r="J133" s="1">
+        <v>0.82663621224767481</v>
+      </c>
+      <c r="K133" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <v>1984</v>
+      </c>
+      <c r="B134" s="1">
+        <v>0.90820849064545039</v>
+      </c>
+      <c r="C134" s="1">
+        <v>0.74657795557602713</v>
+      </c>
+      <c r="D134" s="1">
+        <v>0.98529205785700735</v>
+      </c>
+      <c r="E134" s="1">
+        <v>0.15348789171145882</v>
+      </c>
+      <c r="F134" s="1">
+        <v>0.28448825158327801</v>
+      </c>
+      <c r="G134" s="1">
+        <v>0.75782783828495426</v>
+      </c>
+      <c r="H134" s="1">
+        <v>1</v>
+      </c>
+      <c r="I134" s="1">
+        <v>0.72117780262176734</v>
+      </c>
+      <c r="J134" s="1">
+        <v>0.83070215478585041</v>
+      </c>
+      <c r="K134" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
+        <v>1985</v>
+      </c>
+      <c r="B135" s="1">
+        <v>0.90636342117232249</v>
+      </c>
+      <c r="C135" s="1">
+        <v>0.74684475520235416</v>
+      </c>
+      <c r="D135" s="1">
+        <v>0.98617062950972556</v>
+      </c>
+      <c r="E135" s="1">
+        <v>0.15011736237589715</v>
+      </c>
+      <c r="F135" s="1">
+        <v>0.29421895173682888</v>
+      </c>
+      <c r="G135" s="1">
+        <v>0.74905766437955834</v>
+      </c>
+      <c r="H135" s="1">
+        <v>1</v>
+      </c>
+      <c r="I135" s="1">
+        <v>0.72129424470563885</v>
+      </c>
+      <c r="J135" s="1">
+        <v>0.8376827464544857</v>
+      </c>
+      <c r="K135" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A136" s="1">
+        <v>1986</v>
+      </c>
+      <c r="B136" s="1">
+        <v>0.90360612953650332</v>
+      </c>
+      <c r="C136" s="1">
+        <v>0.72967409204452305</v>
+      </c>
+      <c r="D136" s="1">
+        <v>0.9884764751210191</v>
+      </c>
+      <c r="E136" s="1">
+        <v>0.15338248746158586</v>
+      </c>
+      <c r="F136" s="1">
+        <v>0.29866072572315772</v>
+      </c>
+      <c r="G136" s="1">
+        <v>0.75025439281733874</v>
+      </c>
+      <c r="H136" s="1">
+        <v>1</v>
+      </c>
+      <c r="I136" s="1">
+        <v>0.71241068663151874</v>
+      </c>
+      <c r="J136" s="1">
+        <v>0.84165063701251908</v>
+      </c>
+      <c r="K136" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A137" s="1">
+        <v>1987</v>
+      </c>
+      <c r="B137" s="1">
+        <v>0.90518313913686432</v>
+      </c>
+      <c r="C137" s="1">
+        <v>0.72348578377860739</v>
+      </c>
+      <c r="D137" s="1">
+        <v>0.98956550814267741</v>
+      </c>
+      <c r="E137" s="1">
+        <v>0.14651974587888644</v>
+      </c>
+      <c r="F137" s="1">
+        <v>0.30371242878261373</v>
+      </c>
+      <c r="G137" s="1">
+        <v>0.74316844080089506</v>
+      </c>
+      <c r="H137" s="1">
+        <v>1</v>
+      </c>
+      <c r="I137" s="1">
+        <v>0.73546853684574687</v>
+      </c>
+      <c r="J137" s="1">
+        <v>0.83607298006017927</v>
+      </c>
+      <c r="K137" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <v>1988</v>
+      </c>
+      <c r="B138" s="1">
+        <v>0.90671069357334111</v>
+      </c>
+      <c r="C138" s="1">
+        <v>0.73191391989613741</v>
+      </c>
+      <c r="D138" s="1">
+        <v>0.98997879284181345</v>
+      </c>
+      <c r="E138" s="1">
+        <v>0.14612196059799823</v>
+      </c>
+      <c r="F138" s="1">
+        <v>0.30838564661245293</v>
+      </c>
+      <c r="G138" s="1">
+        <v>0.81542304792783171</v>
+      </c>
+      <c r="H138" s="1">
+        <v>1</v>
+      </c>
+      <c r="I138" s="1">
+        <v>0.65216962082756846</v>
+      </c>
+      <c r="J138" s="1">
+        <v>0.83339426586180221</v>
+      </c>
+      <c r="K138" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A139" s="1">
+        <v>1989</v>
+      </c>
+      <c r="B139" s="1">
+        <v>0.91014206334438863</v>
+      </c>
+      <c r="C139" s="1">
+        <v>0.7446630004122915</v>
+      </c>
+      <c r="D139" s="1">
+        <v>0.9901292989364272</v>
+      </c>
+      <c r="E139" s="1">
+        <v>0.15065660080197785</v>
+      </c>
+      <c r="F139" s="1">
+        <v>0.3159182144331536</v>
+      </c>
+      <c r="G139" s="1">
+        <v>0.81345833269489898</v>
+      </c>
+      <c r="H139" s="1">
+        <v>1</v>
+      </c>
+      <c r="I139" s="1">
+        <v>0.56708718310888384</v>
+      </c>
+      <c r="J139" s="1">
+        <v>0.83043086671913091</v>
+      </c>
+      <c r="K139" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A140" s="1">
+        <v>1990</v>
+      </c>
+      <c r="B140" s="1">
+        <v>0.90160469454497405</v>
+      </c>
+      <c r="C140" s="1">
+        <v>0.7633303938183339</v>
+      </c>
+      <c r="D140" s="1">
+        <v>0.99042778552559152</v>
+      </c>
+      <c r="E140" s="1">
+        <v>0.1522915199093865</v>
+      </c>
+      <c r="F140" s="1">
+        <v>0.32866744438010287</v>
+      </c>
+      <c r="G140" s="1">
+        <v>0.81947716934436499</v>
+      </c>
+      <c r="H140" s="1">
+        <v>1</v>
+      </c>
+      <c r="I140" s="1">
+        <v>0.60611537750847322</v>
+      </c>
+      <c r="J140" s="1">
+        <v>0.84360877263864975</v>
+      </c>
+      <c r="K140" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <v>1991</v>
+      </c>
+      <c r="B141" s="1">
+        <v>0.89996181930706931</v>
+      </c>
+      <c r="C141" s="1">
+        <v>0.76844402743578188</v>
+      </c>
+      <c r="D141" s="1">
+        <v>0.9910022913153288</v>
+      </c>
+      <c r="E141" s="1">
+        <v>0.15628511276971421</v>
+      </c>
+      <c r="F141" s="1">
+        <v>0.33811448413105272</v>
+      </c>
+      <c r="G141" s="1">
+        <v>0.83146476949298531</v>
+      </c>
+      <c r="H141" s="1">
+        <v>1</v>
+      </c>
+      <c r="I141" s="1">
+        <v>0.58276568277777718</v>
+      </c>
+      <c r="J141" s="1">
+        <v>0.85290665820184586</v>
+      </c>
+      <c r="K141" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A142" s="1">
+        <v>1992</v>
+      </c>
+      <c r="B142" s="1">
+        <v>0.89925563204818171</v>
+      </c>
+      <c r="C142" s="1">
+        <v>0.76793371072363048</v>
+      </c>
+      <c r="D142" s="1">
+        <v>0.99092899805506929</v>
+      </c>
+      <c r="E142" s="1">
+        <v>0.1528944813267204</v>
+      </c>
+      <c r="F142" s="1">
+        <v>0.34113927073267808</v>
+      </c>
+      <c r="G142" s="1">
+        <v>0.82356224512929443</v>
+      </c>
+      <c r="H142" s="1">
+        <v>1</v>
+      </c>
+      <c r="I142" s="1">
+        <v>0.56799105484244827</v>
+      </c>
+      <c r="J142" s="1">
+        <v>0.85081778638075689</v>
+      </c>
+      <c r="K142" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A143" s="1">
+        <v>1993</v>
+      </c>
+      <c r="B143" s="1">
+        <v>0.89442149830324669</v>
+      </c>
+      <c r="C143" s="1">
+        <v>0.7546243657978442</v>
+      </c>
+      <c r="D143" s="1">
+        <v>0.99065139865673613</v>
+      </c>
+      <c r="E143" s="1">
+        <v>0.14241851471488656</v>
+      </c>
+      <c r="F143" s="1">
+        <v>0.33146346179504221</v>
+      </c>
+      <c r="G143" s="1">
+        <v>0.81817796687475741</v>
+      </c>
+      <c r="H143" s="1">
+        <v>1</v>
+      </c>
+      <c r="I143" s="1">
+        <v>0.50287710432088906</v>
+      </c>
+      <c r="J143" s="1">
+        <v>0.8391943634415473</v>
+      </c>
+      <c r="K143" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>1994</v>
+      </c>
+      <c r="B144" s="1">
+        <v>0.89253428445501493</v>
+      </c>
+      <c r="C144" s="1">
+        <v>0.74971132216889047</v>
+      </c>
+      <c r="D144" s="1">
+        <v>0.99039139832991041</v>
+      </c>
+      <c r="E144" s="1">
+        <v>0.13154877814487045</v>
+      </c>
+      <c r="F144" s="1">
+        <v>0.32408889430491683</v>
+      </c>
+      <c r="G144" s="1">
+        <v>0.85496253867000083</v>
+      </c>
+      <c r="H144" s="1">
+        <v>1</v>
+      </c>
+      <c r="I144" s="1">
+        <v>0.48683855368025025</v>
+      </c>
+      <c r="J144" s="1">
+        <v>0.83791891311285038</v>
+      </c>
+      <c r="K144" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>1995</v>
+      </c>
+      <c r="B145" s="1">
+        <v>0.90169782400263665</v>
+      </c>
+      <c r="C145" s="1">
+        <v>0.75465887502208706</v>
+      </c>
+      <c r="D145" s="1">
+        <v>0.98972563130782909</v>
+      </c>
+      <c r="E145" s="1">
+        <v>0.12132562065759785</v>
+      </c>
+      <c r="F145" s="1">
+        <v>0.3303945622883423</v>
+      </c>
+      <c r="G145" s="1">
+        <v>0.80595661355800741</v>
+      </c>
+      <c r="H145" s="1">
+        <v>1</v>
+      </c>
+      <c r="I145" s="1">
+        <v>0.47938697018714554</v>
+      </c>
+      <c r="J145" s="1">
+        <v>0.82258032180078366</v>
+      </c>
+      <c r="K145" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A146" s="1">
+        <v>1996</v>
+      </c>
+      <c r="B146" s="1">
+        <v>0.90727757952961807</v>
+      </c>
+      <c r="C146" s="1">
+        <v>0.75791092193578879</v>
+      </c>
+      <c r="D146" s="1">
+        <v>0.9889096283042178</v>
+      </c>
+      <c r="E146" s="1">
+        <v>0.11343139473130637</v>
+      </c>
+      <c r="F146" s="1">
+        <v>0.31874163857488091</v>
+      </c>
+      <c r="G146" s="1">
+        <v>0.78053738549013396</v>
+      </c>
+      <c r="H146" s="1">
+        <v>1</v>
+      </c>
+      <c r="I146" s="1">
+        <v>0.4686445965832442</v>
+      </c>
+      <c r="J146" s="1">
+        <v>0.82455570942245437</v>
+      </c>
+      <c r="K146" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A147" s="1">
+        <v>1997</v>
+      </c>
+      <c r="B147" s="1">
+        <v>0.90551052314870883</v>
+      </c>
+      <c r="C147" s="1">
+        <v>0.7622070750988551</v>
+      </c>
+      <c r="D147" s="1">
+        <v>0.98919162343440048</v>
+      </c>
+      <c r="E147" s="1">
+        <v>0.10727809072460939</v>
+      </c>
+      <c r="F147" s="1">
+        <v>0.31269992147204656</v>
+      </c>
+      <c r="G147" s="1">
+        <v>0.82830499499504051</v>
+      </c>
+      <c r="H147" s="1">
+        <v>1</v>
+      </c>
+      <c r="I147" s="1">
+        <v>0.48516475507477497</v>
+      </c>
+      <c r="J147" s="1">
+        <v>0.82637968191917655</v>
+      </c>
+      <c r="K147" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A148" s="1">
+        <v>1998</v>
+      </c>
+      <c r="B148" s="1">
+        <v>0.90970136664288836</v>
+      </c>
+      <c r="C148" s="1">
+        <v>0.76442712447774086</v>
+      </c>
+      <c r="D148" s="1">
+        <v>0.98782614924145029</v>
+      </c>
+      <c r="E148" s="1">
+        <v>0.10329939716501062</v>
+      </c>
+      <c r="F148" s="1">
+        <v>0.31749293672202394</v>
+      </c>
+      <c r="G148" s="1">
+        <v>0.81425051953345395</v>
+      </c>
+      <c r="H148" s="1">
+        <v>1</v>
+      </c>
+      <c r="I148" s="1">
+        <v>0.54761438647675742</v>
+      </c>
+      <c r="J148" s="1">
+        <v>0.80371391825999128</v>
+      </c>
+      <c r="K148" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A149" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B149" s="1">
+        <v>0.90903270908658629</v>
+      </c>
+      <c r="C149" s="1">
+        <v>0.75979339142043556</v>
+      </c>
+      <c r="D149" s="1">
+        <v>0.98767269409341696</v>
+      </c>
+      <c r="E149" s="1">
+        <v>0.10383205118782457</v>
+      </c>
+      <c r="F149" s="1">
+        <v>0.33467614142344221</v>
+      </c>
+      <c r="G149" s="1">
+        <v>0.74861194679260123</v>
+      </c>
+      <c r="H149" s="1">
+        <v>1</v>
+      </c>
+      <c r="I149" s="1">
+        <v>0.52113596862146605</v>
+      </c>
+      <c r="J149" s="1">
+        <v>0.79078878423020582</v>
+      </c>
+      <c r="K149" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A150" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B150" s="1">
+        <v>0.91002513569109345</v>
+      </c>
+      <c r="C150" s="1">
+        <v>0.75509194323802697</v>
+      </c>
+      <c r="D150" s="1">
+        <v>0.98673812293335084</v>
+      </c>
+      <c r="E150" s="1">
+        <v>0.1043388905119769</v>
+      </c>
+      <c r="F150" s="1">
+        <v>0.349640613311964</v>
+      </c>
+      <c r="G150" s="1">
+        <v>0.79054462190062236</v>
+      </c>
+      <c r="H150" s="1">
+        <v>1</v>
+      </c>
+      <c r="I150" s="1">
+        <v>0.51303970603235138</v>
+      </c>
+      <c r="J150" s="1">
+        <v>0.79256117427238115</v>
+      </c>
+      <c r="K150" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A151" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B151" s="1">
+        <v>0.90720545007314002</v>
+      </c>
+      <c r="C151" s="1">
+        <v>0.7635722716479314</v>
+      </c>
+      <c r="D151" s="1">
+        <v>0.98950720689420868</v>
+      </c>
+      <c r="E151" s="1">
+        <v>9.6800983933714072E-2</v>
+      </c>
+      <c r="F151" s="1">
+        <v>0.36332032874376474</v>
+      </c>
+      <c r="G151" s="1">
+        <v>0.75851171098587344</v>
+      </c>
+      <c r="H151" s="1">
+        <v>1</v>
+      </c>
+      <c r="I151" s="1">
+        <v>0.46663129115640695</v>
+      </c>
+      <c r="J151" s="1">
+        <v>0.80085485842687898</v>
+      </c>
+      <c r="K151" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A152" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B152" s="1">
+        <v>0.90341236773058708</v>
+      </c>
+      <c r="C152" s="1">
+        <v>0.7597646538458398</v>
+      </c>
+      <c r="D152" s="1">
+        <v>0.98290911583424889</v>
+      </c>
+      <c r="E152" s="1">
+        <v>9.0437412475410414E-2</v>
+      </c>
+      <c r="F152" s="1">
+        <v>0.36955577753651103</v>
+      </c>
+      <c r="G152" s="1">
+        <v>0.7501539358330358</v>
+      </c>
+      <c r="H152" s="1">
+        <v>1</v>
+      </c>
+      <c r="I152" s="1">
+        <v>0.44754854638126479</v>
+      </c>
+      <c r="J152" s="1">
+        <v>0.77760675891014597</v>
+      </c>
+      <c r="K152" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A153" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B153" s="1">
+        <v>0.90811567321284858</v>
+      </c>
+      <c r="C153" s="1">
+        <v>0.7611739920859284</v>
+      </c>
+      <c r="D153" s="1">
+        <v>0.98791943169527885</v>
+      </c>
+      <c r="E153" s="1">
+        <v>8.9227109368412022E-2</v>
+      </c>
+      <c r="F153" s="1">
+        <v>0.37526521774751587</v>
+      </c>
+      <c r="G153" s="1">
+        <v>0.74602951376501225</v>
+      </c>
+      <c r="H153" s="1">
+        <v>1</v>
+      </c>
+      <c r="I153" s="1">
+        <v>0.43909932025837883</v>
+      </c>
+      <c r="J153" s="1">
+        <v>0.77379616598478085</v>
+      </c>
+      <c r="K153" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A154" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B154" s="1">
+        <v>0.90666756497644363</v>
+      </c>
+      <c r="C154" s="1">
+        <v>0.74826272694985496</v>
+      </c>
+      <c r="D154" s="1">
+        <v>0.98657834465010918</v>
+      </c>
+      <c r="E154" s="1">
+        <v>8.4901493183079005E-2</v>
+      </c>
+      <c r="F154" s="1">
+        <v>0.37951368753941084</v>
+      </c>
+      <c r="G154" s="1">
+        <v>0.80054699282348474</v>
+      </c>
+      <c r="H154" s="1">
+        <v>1</v>
+      </c>
+      <c r="I154" s="1">
+        <v>0.43889643386048793</v>
+      </c>
+      <c r="J154" s="1">
+        <v>0.78024002128264336</v>
+      </c>
+      <c r="K154" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A155" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B155" s="1">
+        <v>0.90633918822343817</v>
+      </c>
+      <c r="C155" s="1">
+        <v>0.75517769874525043</v>
+      </c>
+      <c r="D155" s="1">
+        <v>0.98631712692019169</v>
+      </c>
+      <c r="E155" s="1">
+        <v>7.5206459440864418E-2</v>
+      </c>
+      <c r="F155" s="1">
+        <v>0.38453394600105278</v>
+      </c>
+      <c r="G155" s="1">
+        <v>0.7756306925201637</v>
+      </c>
+      <c r="H155" s="1">
+        <v>1</v>
+      </c>
+      <c r="I155" s="1">
+        <v>0.47357414600885783</v>
+      </c>
+      <c r="J155" s="1">
+        <v>0.7797274245135315</v>
+      </c>
+      <c r="K155" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A156" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B156" s="1">
+        <v>0.9089608089335155</v>
+      </c>
+      <c r="C156" s="1">
+        <v>0.7373631068051324</v>
+      </c>
+      <c r="D156" s="1">
+        <v>0.98483583051732515</v>
+      </c>
+      <c r="E156" s="1">
+        <v>7.4591937342497805E-2</v>
+      </c>
+      <c r="F156" s="1">
+        <v>0.38269487921344097</v>
+      </c>
+      <c r="G156" s="1">
+        <v>0.71618714061323641</v>
+      </c>
+      <c r="H156" s="1">
+        <v>1</v>
+      </c>
+      <c r="I156" s="1">
+        <v>0.48331982139195845</v>
+      </c>
+      <c r="J156" s="1">
+        <v>0.77729705158342965</v>
+      </c>
+      <c r="K156" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A157" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B157" s="1">
+        <v>0.91059613541733531</v>
+      </c>
+      <c r="C157" s="1">
+        <v>0.73067324992375426</v>
+      </c>
+      <c r="D157" s="1">
+        <v>0.98866795507118166</v>
+      </c>
+      <c r="E157" s="1">
+        <v>7.597063745286918E-2</v>
+      </c>
+      <c r="F157" s="1">
+        <v>0.38405329098001711</v>
+      </c>
+      <c r="G157" s="1">
+        <v>0.78624306856051629</v>
+      </c>
+      <c r="H157" s="1">
+        <v>1</v>
+      </c>
+      <c r="I157" s="1">
+        <v>0.47562750834854089</v>
+      </c>
+      <c r="J157" s="1">
+        <v>0.7846108613424766</v>
+      </c>
+      <c r="K157" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A158" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B158" s="1">
+        <v>0.91067292952291179</v>
+      </c>
+      <c r="C158" s="1">
+        <v>0.72880742062129911</v>
+      </c>
+      <c r="D158" s="1">
+        <v>0.9835849142731633</v>
+      </c>
+      <c r="E158" s="1">
+        <v>7.8906089102032062E-2</v>
+      </c>
+      <c r="F158" s="1">
+        <v>0.38506940487782287</v>
+      </c>
+      <c r="G158" s="1">
+        <v>0.82781367956575613</v>
+      </c>
+      <c r="H158" s="1">
+        <v>1</v>
+      </c>
+      <c r="I158" s="1">
+        <v>0.44048220321895198</v>
+      </c>
+      <c r="J158" s="1">
+        <v>0.80379855419033441</v>
+      </c>
+      <c r="K158" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A159" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B159" s="1">
+        <v>0.90880940551033362</v>
+      </c>
+      <c r="C159" s="1">
+        <v>0.72411711836001025</v>
+      </c>
+      <c r="D159" s="1">
+        <v>0.98450648799315754</v>
+      </c>
+      <c r="E159" s="1">
+        <v>8.4261916689836361E-2</v>
+      </c>
+      <c r="F159" s="1">
+        <v>0.38921556028994853</v>
+      </c>
+      <c r="G159" s="1">
+        <v>0.82680142862198513</v>
+      </c>
+      <c r="H159" s="1">
+        <v>1</v>
+      </c>
+      <c r="I159" s="1">
+        <v>0.44396548255646429</v>
+      </c>
+      <c r="J159" s="1">
+        <v>0.80722348577800307</v>
+      </c>
+      <c r="K159" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A160" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B160" s="1">
+        <v>0.90929130411428283</v>
+      </c>
+      <c r="C160" s="1">
+        <v>0.72070703267127911</v>
+      </c>
+      <c r="D160" s="1">
+        <v>0.98936953468338851</v>
+      </c>
+      <c r="E160" s="1">
+        <v>9.0262622724384886E-2</v>
+      </c>
+      <c r="F160" s="1">
+        <v>0.36215115542800269</v>
+      </c>
+      <c r="G160" s="1">
+        <v>0.79635026541357046</v>
+      </c>
+      <c r="H160" s="1">
+        <v>1</v>
+      </c>
+      <c r="I160" s="1">
+        <v>0.42467272643224319</v>
+      </c>
+      <c r="J160" s="1">
+        <v>0.76148652925145022</v>
+      </c>
+      <c r="K160" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A161" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B161" s="1">
+        <v>0.91146562101119621</v>
+      </c>
+      <c r="C161" s="1">
+        <v>0.72033724606132499</v>
+      </c>
+      <c r="D161" s="1">
+        <v>0.986650067575499</v>
+      </c>
+      <c r="E161" s="1">
+        <v>9.2253724657423306E-2</v>
+      </c>
+      <c r="F161" s="1">
+        <v>0.36320136142890869</v>
+      </c>
+      <c r="G161" s="1">
+        <v>0.79373034133937215</v>
+      </c>
+      <c r="H161" s="1">
+        <v>1</v>
+      </c>
+      <c r="I161" s="1">
+        <v>0.40838444812976504</v>
+      </c>
+      <c r="J161" s="1">
+        <v>0.75531367017463746</v>
+      </c>
+      <c r="K161" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A162" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B162" s="1">
+        <v>0.9087041479536877</v>
+      </c>
+      <c r="C162" s="1">
+        <v>0.7158756884215719</v>
+      </c>
+      <c r="D162" s="1">
+        <v>0.98511818179955513</v>
+      </c>
+      <c r="E162" s="1">
+        <v>9.2691411979801616E-2</v>
+      </c>
+      <c r="F162" s="1">
+        <v>0.36033342667903634</v>
+      </c>
+      <c r="G162" s="1">
+        <v>0.79054593970017517</v>
+      </c>
+      <c r="H162" s="1">
+        <v>1</v>
+      </c>
+      <c r="I162" s="1">
+        <v>0.42808472098296341</v>
+      </c>
+      <c r="J162" s="1">
+        <v>0.7620658070373989</v>
+      </c>
+      <c r="K162" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A163" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B163" s="1">
+        <v>0.90551598703264535</v>
+      </c>
+      <c r="C163" s="1">
+        <v>0.7081791879357906</v>
+      </c>
+      <c r="D163" s="1">
+        <v>0.98752754151078481</v>
+      </c>
+      <c r="E163" s="1">
+        <v>8.9504671719578585E-2</v>
+      </c>
+      <c r="F163" s="1">
+        <v>0.36064311020823175</v>
+      </c>
+      <c r="G163" s="1">
+        <v>0.84338595387674031</v>
+      </c>
+      <c r="H163" s="1">
+        <v>1</v>
+      </c>
+      <c r="I163" s="1">
+        <v>0.42260255628017473</v>
+      </c>
+      <c r="J163" s="1">
+        <v>0.7402150001293184</v>
+      </c>
+      <c r="K163" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A164" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B164" s="1">
+        <v>0.90485621806993644</v>
+      </c>
+      <c r="C164" s="1">
+        <v>0.70375909802917658</v>
+      </c>
+      <c r="D164" s="1">
+        <v>0.98749733684050411</v>
+      </c>
+      <c r="E164" s="1">
+        <v>8.8063925052477593E-2</v>
+      </c>
+      <c r="F164" s="1">
+        <v>0.36339533290921006</v>
+      </c>
+      <c r="G164" s="1">
+        <v>0.83203289070919428</v>
+      </c>
+      <c r="H164" s="1">
+        <v>1</v>
+      </c>
+      <c r="I164" s="1">
+        <v>0.42552814397506039</v>
+      </c>
+      <c r="J164" s="1">
+        <v>0.74200090421129905</v>
+      </c>
+      <c r="K164" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A165" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B165" s="1">
+        <v>0.90394188241631368</v>
+      </c>
+      <c r="C165" s="1">
+        <v>0.70287943391465191</v>
+      </c>
+      <c r="D165" s="1">
+        <v>0.98677482551733886</v>
+      </c>
+      <c r="E165" s="1">
+        <v>8.8410547135578679E-2</v>
+      </c>
+      <c r="F165" s="1">
+        <v>0.3659652251654219</v>
+      </c>
+      <c r="G165" s="1">
+        <v>0.82051153118366194</v>
+      </c>
+      <c r="H165" s="1">
+        <v>1</v>
+      </c>
+      <c r="I165" s="1">
+        <v>0.4293491207847332</v>
+      </c>
+      <c r="J165" s="1">
+        <v>0.73956513583779993</v>
+      </c>
+      <c r="K165" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made filters for each use of funds work
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -395,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="B125" sqref="B125:J165"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3324,34 +3324,34 @@
         <v>1975</v>
       </c>
       <c r="B84" s="1">
-        <v>5.8311674402625122E-2</v>
+        <v>94.168832559737496</v>
       </c>
       <c r="C84" s="1">
-        <v>0.29187722583635556</v>
+        <v>70.812277416364438</v>
       </c>
       <c r="D84" s="1">
-        <v>1.4547206492870602E-2</v>
+        <v>98.545279350712946</v>
       </c>
       <c r="E84" s="1">
-        <v>0.87322180962812435</v>
+        <v>12.677819037187559</v>
       </c>
       <c r="F84" s="1">
-        <v>0.85281657418091961</v>
+        <v>14.718342581908036</v>
       </c>
       <c r="G84" s="1">
-        <v>0.29780221585255545</v>
+        <v>70.219778414744454</v>
       </c>
       <c r="H84" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I84" s="1">
-        <v>0.21014334660824266</v>
+        <v>78.985665339175739</v>
       </c>
       <c r="J84" s="1">
-        <v>0.36957154380133234</v>
+        <v>63.042845619866775</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
@@ -3359,34 +3359,34 @@
         <v>1976</v>
       </c>
       <c r="B85" s="1">
-        <v>5.971407867671253E-2</v>
+        <v>94.02859213232874</v>
       </c>
       <c r="C85" s="1">
-        <v>0.27000023256856143</v>
+        <v>72.999976743143861</v>
       </c>
       <c r="D85" s="1">
-        <v>1.424961388890846E-2</v>
+        <v>98.57503861110915</v>
       </c>
       <c r="E85" s="1">
-        <v>0.87104442973774743</v>
+        <v>12.89555702622525</v>
       </c>
       <c r="F85" s="1">
-        <v>0.82004863600648392</v>
+        <v>17.995136399351605</v>
       </c>
       <c r="G85" s="1">
-        <v>0.32554461428488857</v>
+        <v>67.445538571511136</v>
       </c>
       <c r="H85" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I85" s="1">
-        <v>0.17136777705756526</v>
+        <v>82.863222294243471</v>
       </c>
       <c r="J85" s="1">
-        <v>0.33383308027367142</v>
+        <v>66.61669197263285</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
@@ -3394,34 +3394,34 @@
         <v>1977</v>
       </c>
       <c r="B86" s="1">
-        <v>6.18472651901118E-2</v>
+        <v>93.815273480988822</v>
       </c>
       <c r="C86" s="1">
-        <v>0.25479181025267117</v>
+        <v>74.52081897473289</v>
       </c>
       <c r="D86" s="1">
-        <v>1.4138017779323921E-2</v>
+        <v>98.586198222067623</v>
       </c>
       <c r="E86" s="1">
-        <v>0.87334656989073445</v>
+        <v>12.665343010926552</v>
       </c>
       <c r="F86" s="1">
-        <v>0.79689491756169117</v>
+        <v>20.310508243830888</v>
       </c>
       <c r="G86" s="1">
-        <v>0.31627580951960121</v>
+        <v>68.372419048039873</v>
       </c>
       <c r="H86" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I86" s="1">
-        <v>0.22083505828289887</v>
+        <v>77.916494171710113</v>
       </c>
       <c r="J86" s="1">
-        <v>0.31671702238106852</v>
+        <v>68.328297761893154</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
@@ -3429,34 +3429,34 @@
         <v>1978</v>
       </c>
       <c r="B87" s="1">
-        <v>7.0453570058374451E-2</v>
+        <v>92.954642994162555</v>
       </c>
       <c r="C87" s="1">
-        <v>0.26154395704080347</v>
+        <v>73.845604295919657</v>
       </c>
       <c r="D87" s="1">
-        <v>1.4937134834398668E-2</v>
+        <v>98.506286516560124</v>
       </c>
       <c r="E87" s="1">
-        <v>0.86496068774440094</v>
+        <v>13.503931225559903</v>
       </c>
       <c r="F87" s="1">
-        <v>0.77312928370429079</v>
+        <v>22.687071629570912</v>
       </c>
       <c r="G87" s="1">
-        <v>0.32339277204319933</v>
+        <v>67.660722795680059</v>
       </c>
       <c r="H87" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I87" s="1">
-        <v>0.21184037016623886</v>
+        <v>78.815962983376124</v>
       </c>
       <c r="J87" s="1">
-        <v>0.265562429624422</v>
+        <v>73.443757037557802</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
@@ -3464,34 +3464,34 @@
         <v>1979</v>
       </c>
       <c r="B88" s="1">
-        <v>7.7214376853833797E-2</v>
+        <v>92.278562314616622</v>
       </c>
       <c r="C88" s="1">
-        <v>0.27182954471189458</v>
+        <v>72.817045528810539</v>
       </c>
       <c r="D88" s="1">
-        <v>1.8399164988687149E-2</v>
+        <v>98.160083501131282</v>
       </c>
       <c r="E88" s="1">
-        <v>0.85164648196923221</v>
+        <v>14.835351803076788</v>
       </c>
       <c r="F88" s="1">
-        <v>0.76700035147921031</v>
+        <v>23.299964852078975</v>
       </c>
       <c r="G88" s="1">
-        <v>0.24454412914741749</v>
+        <v>75.545587085258248</v>
       </c>
       <c r="H88" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I88" s="1">
-        <v>0.22154753504298669</v>
+        <v>77.845246495701332</v>
       </c>
       <c r="J88" s="1">
-        <v>0.24718662783418749</v>
+        <v>75.28133721658125</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
@@ -3499,34 +3499,34 @@
         <v>1980</v>
       </c>
       <c r="B89" s="1">
-        <v>8.0263776539113874E-2</v>
+        <v>91.973622346088618</v>
       </c>
       <c r="C89" s="1">
-        <v>0.28278186759612689</v>
+        <v>71.72181324038732</v>
       </c>
       <c r="D89" s="1">
-        <v>1.5675392437735122E-2</v>
+        <v>98.43246075622649</v>
       </c>
       <c r="E89" s="1">
-        <v>0.83770367426750303</v>
+        <v>16.229632573249688</v>
       </c>
       <c r="F89" s="1">
-        <v>0.75326436769519722</v>
+        <v>24.673563230480276</v>
       </c>
       <c r="G89" s="1">
-        <v>0.35876794949276103</v>
+        <v>64.123205050723897</v>
       </c>
       <c r="H89" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I89" s="1">
-        <v>0.22858775239505263</v>
+        <v>77.141224760494737</v>
       </c>
       <c r="J89" s="1">
-        <v>0.23483481407781481</v>
+        <v>76.516518592218517</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
@@ -3534,34 +3534,34 @@
         <v>1981</v>
       </c>
       <c r="B90" s="1">
-        <v>8.1895472225121183E-2</v>
+        <v>91.810452777487882</v>
       </c>
       <c r="C90" s="1">
-        <v>0.2571728251483556</v>
+        <v>74.28271748516444</v>
       </c>
       <c r="D90" s="1">
-        <v>1.2999820449641149E-2</v>
+        <v>98.700017955035875</v>
       </c>
       <c r="E90" s="1">
-        <v>0.81596041662722507</v>
+        <v>18.403958337277494</v>
       </c>
       <c r="F90" s="1">
-        <v>0.75692532956738434</v>
+        <v>24.307467043261564</v>
       </c>
       <c r="G90" s="1">
-        <v>0.34133186682709471</v>
+        <v>65.866813317290536</v>
       </c>
       <c r="H90" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I90" s="1">
-        <v>0.2952981013123227</v>
+        <v>70.470189868767719</v>
       </c>
       <c r="J90" s="1">
-        <v>0.19678893184570076</v>
+        <v>80.321106815429914</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
@@ -3569,34 +3569,34 @@
         <v>1982</v>
       </c>
       <c r="B91" s="1">
-        <v>8.3315721911614959E-2</v>
+        <v>91.668427808838501</v>
       </c>
       <c r="C91" s="1">
-        <v>0.25213662517000351</v>
+        <v>74.786337482999656</v>
       </c>
       <c r="D91" s="1">
-        <v>1.5304954549127397E-2</v>
+        <v>98.469504545087261</v>
       </c>
       <c r="E91" s="1">
-        <v>0.83414439005336405</v>
+        <v>16.585560994663588</v>
       </c>
       <c r="F91" s="1">
-        <v>0.74097426656966636</v>
+        <v>25.902573343033364</v>
       </c>
       <c r="G91" s="1">
-        <v>0.35067881892554842</v>
+        <v>64.932118107445163</v>
       </c>
       <c r="H91" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I91" s="1">
-        <v>0.21152603434538431</v>
+        <v>78.84739656546158</v>
       </c>
       <c r="J91" s="1">
-        <v>0.18370591448026152</v>
+        <v>81.629408551973853</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
@@ -3604,34 +3604,34 @@
         <v>1983</v>
       </c>
       <c r="B92" s="1">
-        <v>8.6219175981053192E-2</v>
+        <v>91.378082401894687</v>
       </c>
       <c r="C92" s="1">
-        <v>0.25315431718821618</v>
+        <v>74.684568281178386</v>
       </c>
       <c r="D92" s="1">
-        <v>1.571267381136374E-2</v>
+        <v>98.42873261886362</v>
       </c>
       <c r="E92" s="1">
-        <v>0.84180530901786521</v>
+        <v>15.819469098213478</v>
       </c>
       <c r="F92" s="1">
-        <v>0.72320657267242594</v>
+        <v>27.679342732757402</v>
       </c>
       <c r="G92" s="1">
-        <v>0.25850095958645619</v>
+        <v>74.149904041354375</v>
       </c>
       <c r="H92" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I92" s="1">
-        <v>0.2261678094629396</v>
+        <v>77.383219053706043</v>
       </c>
       <c r="J92" s="1">
-        <v>0.1733637877523253</v>
+        <v>82.663621224767482</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
@@ -3639,34 +3639,34 @@
         <v>1984</v>
       </c>
       <c r="B93" s="1">
-        <v>9.1791509354549522E-2</v>
+        <v>90.820849064545044</v>
       </c>
       <c r="C93" s="1">
-        <v>0.25342204442397287</v>
+        <v>74.657795557602711</v>
       </c>
       <c r="D93" s="1">
-        <v>1.4707942142992715E-2</v>
+        <v>98.529205785700739</v>
       </c>
       <c r="E93" s="1">
-        <v>0.84651210828854118</v>
+        <v>15.348789171145881</v>
       </c>
       <c r="F93" s="1">
-        <v>0.71551174841672205</v>
+        <v>28.4488251583278</v>
       </c>
       <c r="G93" s="1">
-        <v>0.24217216171504583</v>
+        <v>75.782783828495425</v>
       </c>
       <c r="H93" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I93" s="1">
-        <v>0.27882219737823266</v>
+        <v>72.117780262176737</v>
       </c>
       <c r="J93" s="1">
-        <v>0.16929784521414953</v>
+        <v>83.070215478585041</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
@@ -3674,34 +3674,34 @@
         <v>1985</v>
       </c>
       <c r="B94" s="1">
-        <v>9.3636578827677605E-2</v>
+        <v>90.636342117232246</v>
       </c>
       <c r="C94" s="1">
-        <v>0.2531552447976459</v>
+        <v>74.684475520235409</v>
       </c>
       <c r="D94" s="1">
-        <v>1.3829370490274351E-2</v>
+        <v>98.617062950972553</v>
       </c>
       <c r="E94" s="1">
-        <v>0.84988263762410288</v>
+        <v>15.011736237589716</v>
       </c>
       <c r="F94" s="1">
-        <v>0.70578104826317112</v>
+        <v>29.421895173682888</v>
       </c>
       <c r="G94" s="1">
-        <v>0.25094233562044166</v>
+        <v>74.905766437955833</v>
       </c>
       <c r="H94" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I94" s="1">
-        <v>0.2787057552943612</v>
+        <v>72.12942447056389</v>
       </c>
       <c r="J94" s="1">
-        <v>0.16231725354551427</v>
+        <v>83.768274645448571</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
@@ -3709,34 +3709,34 @@
         <v>1986</v>
       </c>
       <c r="B95" s="1">
-        <v>9.6393870463496636E-2</v>
+        <v>90.360612953650332</v>
       </c>
       <c r="C95" s="1">
-        <v>0.27032590795547684</v>
+        <v>72.967409204452309</v>
       </c>
       <c r="D95" s="1">
-        <v>1.1523524878980885E-2</v>
+        <v>98.847647512101915</v>
       </c>
       <c r="E95" s="1">
-        <v>0.84661751253841411</v>
+        <v>15.338248746158586</v>
       </c>
       <c r="F95" s="1">
-        <v>0.70133927427684217</v>
+        <v>29.866072572315773</v>
       </c>
       <c r="G95" s="1">
-        <v>0.24974560718266123</v>
+        <v>75.025439281733881</v>
       </c>
       <c r="H95" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I95" s="1">
-        <v>0.28758931336848126</v>
+        <v>71.241068663151879</v>
       </c>
       <c r="J95" s="1">
-        <v>0.1583493629874809</v>
+        <v>84.16506370125191</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
@@ -3744,34 +3744,34 @@
         <v>1987</v>
       </c>
       <c r="B96" s="1">
-        <v>9.4816860863135718E-2</v>
+        <v>90.518313913686427</v>
       </c>
       <c r="C96" s="1">
-        <v>0.27651421622139266</v>
+        <v>72.348578377860733</v>
       </c>
       <c r="D96" s="1">
-        <v>1.0434491857322576E-2</v>
+        <v>98.956550814267743</v>
       </c>
       <c r="E96" s="1">
-        <v>0.85348025412111361</v>
+        <v>14.651974587888644</v>
       </c>
       <c r="F96" s="1">
-        <v>0.69628757121738627</v>
+        <v>30.371242878261373</v>
       </c>
       <c r="G96" s="1">
-        <v>0.25683155919910494</v>
+        <v>74.31684408008951</v>
       </c>
       <c r="H96" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I96" s="1">
-        <v>0.26453146315425313</v>
+        <v>73.546853684574685</v>
       </c>
       <c r="J96" s="1">
-        <v>0.16392701993982073</v>
+        <v>83.607298006017928</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
@@ -3779,34 +3779,34 @@
         <v>1988</v>
       </c>
       <c r="B97" s="1">
-        <v>9.3289306426658808E-2</v>
+        <v>90.671069357334105</v>
       </c>
       <c r="C97" s="1">
-        <v>0.26808608010386253</v>
+        <v>73.191391989613734</v>
       </c>
       <c r="D97" s="1">
-        <v>1.0021207158186565E-2</v>
+        <v>98.997879284181352</v>
       </c>
       <c r="E97" s="1">
-        <v>0.8538780394020018</v>
+        <v>14.612196059799823</v>
       </c>
       <c r="F97" s="1">
-        <v>0.69161435338754695</v>
+        <v>30.838564661245293</v>
       </c>
       <c r="G97" s="1">
-        <v>0.18457695207216826</v>
+        <v>81.54230479278317</v>
       </c>
       <c r="H97" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I97" s="1">
-        <v>0.34783037917243154</v>
+        <v>65.216962082756851</v>
       </c>
       <c r="J97" s="1">
-        <v>0.16660573413819771</v>
+        <v>83.339426586180224</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
@@ -3814,34 +3814,34 @@
         <v>1989</v>
       </c>
       <c r="B98" s="1">
-        <v>8.9857936655611315E-2</v>
+        <v>91.014206334438867</v>
       </c>
       <c r="C98" s="1">
-        <v>0.2553369995877085</v>
+        <v>74.466300041229147</v>
       </c>
       <c r="D98" s="1">
-        <v>9.8707010635727122E-3</v>
+        <v>99.01292989364272</v>
       </c>
       <c r="E98" s="1">
-        <v>0.84934339919802204</v>
+        <v>15.065660080197784</v>
       </c>
       <c r="F98" s="1">
-        <v>0.6840817855668464</v>
+        <v>31.591821443315361</v>
       </c>
       <c r="G98" s="1">
-        <v>0.18654166730510111</v>
+        <v>81.345833269489901</v>
       </c>
       <c r="H98" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I98" s="1">
-        <v>0.43291281689111605</v>
+        <v>56.708718310888386</v>
       </c>
       <c r="J98" s="1">
-        <v>0.16956913328086914</v>
+        <v>83.043086671913088</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
@@ -3849,34 +3849,34 @@
         <v>1990</v>
       </c>
       <c r="B99" s="1">
-        <v>9.8395305455026033E-2</v>
+        <v>90.160469454497402</v>
       </c>
       <c r="C99" s="1">
-        <v>0.23666960618166608</v>
+        <v>76.333039381833387</v>
       </c>
       <c r="D99" s="1">
-        <v>9.5722144744084681E-3</v>
+        <v>99.042778552559156</v>
       </c>
       <c r="E99" s="1">
-        <v>0.8477084800906135</v>
+        <v>15.22915199093865</v>
       </c>
       <c r="F99" s="1">
-        <v>0.67133255561989702</v>
+        <v>32.866744438010286</v>
       </c>
       <c r="G99" s="1">
-        <v>0.18052283065563499</v>
+        <v>81.9477169344365</v>
       </c>
       <c r="H99" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I99" s="1">
-        <v>0.39388462249152678</v>
+        <v>60.611537750847319</v>
       </c>
       <c r="J99" s="1">
-        <v>0.15639122736135017</v>
+        <v>84.360877263864978</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
@@ -3884,34 +3884,34 @@
         <v>1991</v>
       </c>
       <c r="B100" s="1">
-        <v>0.1000381806929307</v>
+        <v>89.996181930706925</v>
       </c>
       <c r="C100" s="1">
-        <v>0.23155597256421806</v>
+        <v>76.844402743578186</v>
       </c>
       <c r="D100" s="1">
-        <v>8.9977086846712451E-3</v>
+        <v>99.100229131532885</v>
       </c>
       <c r="E100" s="1">
-        <v>0.84371488723028576</v>
+        <v>15.628511276971421</v>
       </c>
       <c r="F100" s="1">
-        <v>0.66188551586894728</v>
+        <v>33.811448413105275</v>
       </c>
       <c r="G100" s="1">
-        <v>0.16853523050701466</v>
+        <v>83.146476949298531</v>
       </c>
       <c r="H100" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I100" s="1">
-        <v>0.41723431722222276</v>
+        <v>58.27656827777772</v>
       </c>
       <c r="J100" s="1">
-        <v>0.14709334179815414</v>
+        <v>85.290665820184586</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
@@ -3919,34 +3919,34 @@
         <v>1992</v>
       </c>
       <c r="B101" s="1">
-        <v>0.10074436795181826</v>
+        <v>89.925563204818175</v>
       </c>
       <c r="C101" s="1">
-        <v>0.23206628927636958</v>
+        <v>76.793371072363044</v>
       </c>
       <c r="D101" s="1">
-        <v>9.0710019449306255E-3</v>
+        <v>99.092899805506931</v>
       </c>
       <c r="E101" s="1">
-        <v>0.84710551867327955</v>
+        <v>15.289448132672041</v>
       </c>
       <c r="F101" s="1">
-        <v>0.65886072926732198</v>
+        <v>34.11392707326781</v>
       </c>
       <c r="G101" s="1">
-        <v>0.17643775487070562</v>
+        <v>82.356224512929444</v>
       </c>
       <c r="H101" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I101" s="1">
-        <v>0.43200894515755178</v>
+        <v>56.799105484244826</v>
       </c>
       <c r="J101" s="1">
-        <v>0.14918221361924303</v>
+        <v>85.08177863807569</v>
       </c>
       <c r="K101" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
@@ -3954,34 +3954,34 @@
         <v>1993</v>
       </c>
       <c r="B102" s="1">
-        <v>0.10557850169675322</v>
+        <v>89.442149830324666</v>
       </c>
       <c r="C102" s="1">
-        <v>0.24537563420215591</v>
+        <v>75.462436579784423</v>
       </c>
       <c r="D102" s="1">
-        <v>9.3486013432638841E-3</v>
+        <v>99.065139865673615</v>
       </c>
       <c r="E102" s="1">
-        <v>0.85758148528511335</v>
+        <v>14.241851471488657</v>
       </c>
       <c r="F102" s="1">
-        <v>0.66853653820495784</v>
+        <v>33.146346179504221</v>
       </c>
       <c r="G102" s="1">
-        <v>0.18182203312524259</v>
+        <v>81.817796687475735</v>
       </c>
       <c r="H102" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I102" s="1">
-        <v>0.49712289567911089</v>
+        <v>50.287710432088907</v>
       </c>
       <c r="J102" s="1">
-        <v>0.16080563655845276</v>
+        <v>83.919436344154732</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
@@ -3989,34 +3989,34 @@
         <v>1994</v>
       </c>
       <c r="B103" s="1">
-        <v>0.107465715544985</v>
+        <v>89.253428445501498</v>
       </c>
       <c r="C103" s="1">
-        <v>0.25028867783110959</v>
+        <v>74.971132216889046</v>
       </c>
       <c r="D103" s="1">
-        <v>9.6086016700896067E-3</v>
+        <v>99.03913983299104</v>
       </c>
       <c r="E103" s="1">
-        <v>0.86845122185512957</v>
+        <v>13.154877814487046</v>
       </c>
       <c r="F103" s="1">
-        <v>0.67591110569508317</v>
+        <v>32.408889430491683</v>
       </c>
       <c r="G103" s="1">
-        <v>0.14503746132999917</v>
+        <v>85.496253867000078</v>
       </c>
       <c r="H103" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I103" s="1">
-        <v>0.51316144631974958</v>
+        <v>48.683855368025029</v>
       </c>
       <c r="J103" s="1">
-        <v>0.16208108688714953</v>
+        <v>83.791891311285042</v>
       </c>
       <c r="K103" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
@@ -4024,34 +4024,34 @@
         <v>1995</v>
       </c>
       <c r="B104" s="1">
-        <v>9.8302175997363461E-2</v>
+        <v>90.169782400263671</v>
       </c>
       <c r="C104" s="1">
-        <v>0.24534112497791302</v>
+        <v>75.465887502208702</v>
       </c>
       <c r="D104" s="1">
-        <v>1.0274368692170913E-2</v>
+        <v>98.972563130782902</v>
       </c>
       <c r="E104" s="1">
-        <v>0.87867437934240211</v>
+        <v>12.132562065759785</v>
       </c>
       <c r="F104" s="1">
-        <v>0.66960543771165781</v>
+        <v>33.039456228834233</v>
       </c>
       <c r="G104" s="1">
-        <v>0.19404338644199262</v>
+        <v>80.595661355800743</v>
       </c>
       <c r="H104" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I104" s="1">
-        <v>0.52061302981285451</v>
+        <v>47.938697018714556</v>
       </c>
       <c r="J104" s="1">
-        <v>0.17741967819921628</v>
+        <v>82.258032180078374</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
@@ -4059,34 +4059,34 @@
         <v>1996</v>
       </c>
       <c r="B105" s="1">
-        <v>9.2722420470381872E-2</v>
+        <v>90.727757952961809</v>
       </c>
       <c r="C105" s="1">
-        <v>0.24208907806421121</v>
+        <v>75.791092193578876</v>
       </c>
       <c r="D105" s="1">
-        <v>1.10903716957821E-2</v>
+        <v>98.890962830421785</v>
       </c>
       <c r="E105" s="1">
-        <v>0.88656860526869363</v>
+        <v>11.343139473130638</v>
       </c>
       <c r="F105" s="1">
-        <v>0.68125836142511909</v>
+        <v>31.874163857488092</v>
       </c>
       <c r="G105" s="1">
-        <v>0.21946261450986604</v>
+        <v>78.053738549013403</v>
       </c>
       <c r="H105" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I105" s="1">
-        <v>0.53135540341675591</v>
+        <v>46.864459658324421</v>
       </c>
       <c r="J105" s="1">
-        <v>0.17544429057754568</v>
+        <v>82.455570942245444</v>
       </c>
       <c r="K105" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
@@ -4094,34 +4094,34 @@
         <v>1997</v>
       </c>
       <c r="B106" s="1">
-        <v>9.4489476851291179E-2</v>
+        <v>90.551052314870887</v>
       </c>
       <c r="C106" s="1">
-        <v>0.23779292490114481</v>
+        <v>76.220707509885514</v>
       </c>
       <c r="D106" s="1">
-        <v>1.080837656559961E-2</v>
+        <v>98.91916234344005</v>
       </c>
       <c r="E106" s="1">
-        <v>0.89272190927539075</v>
+        <v>10.727809072460939</v>
       </c>
       <c r="F106" s="1">
-        <v>0.68730007852795338</v>
+        <v>31.269992147204658</v>
       </c>
       <c r="G106" s="1">
-        <v>0.17169500500495946</v>
+        <v>82.830499499504057</v>
       </c>
       <c r="H106" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I106" s="1">
-        <v>0.51483524492522503</v>
+        <v>48.516475507477494</v>
       </c>
       <c r="J106" s="1">
-        <v>0.17362031808082345</v>
+        <v>82.637968191917651</v>
       </c>
       <c r="K106" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
@@ -4129,34 +4129,34 @@
         <v>1998</v>
       </c>
       <c r="B107" s="1">
-        <v>9.029863335711158E-2</v>
+        <v>90.97013666428883</v>
       </c>
       <c r="C107" s="1">
-        <v>0.23557287552225917</v>
+        <v>76.442712447774085</v>
       </c>
       <c r="D107" s="1">
-        <v>1.2173850758549662E-2</v>
+        <v>98.782614924145022</v>
       </c>
       <c r="E107" s="1">
-        <v>0.89670060283498942</v>
+        <v>10.329939716501062</v>
       </c>
       <c r="F107" s="1">
-        <v>0.68250706327797617</v>
+        <v>31.749293672202395</v>
       </c>
       <c r="G107" s="1">
-        <v>0.18574948046654599</v>
+        <v>81.425051953345388</v>
       </c>
       <c r="H107" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I107" s="1">
-        <v>0.45238561352324258</v>
+        <v>54.761438647675739</v>
       </c>
       <c r="J107" s="1">
-        <v>0.19628608174000883</v>
+        <v>80.371391825999126</v>
       </c>
       <c r="K107" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
@@ -4164,34 +4164,34 @@
         <v>1999</v>
       </c>
       <c r="B108" s="1">
-        <v>9.0967290913413656E-2</v>
+        <v>90.903270908658627</v>
       </c>
       <c r="C108" s="1">
-        <v>0.24020660857956433</v>
+        <v>75.979339142043557</v>
       </c>
       <c r="D108" s="1">
-        <v>1.2327305906583139E-2</v>
+        <v>98.767269409341694</v>
       </c>
       <c r="E108" s="1">
-        <v>0.89616794881217543</v>
+        <v>10.383205118782456</v>
       </c>
       <c r="F108" s="1">
-        <v>0.66532385857655785</v>
+        <v>33.467614142344217</v>
       </c>
       <c r="G108" s="1">
-        <v>0.25138805320739871</v>
+        <v>74.861194679260123</v>
       </c>
       <c r="H108" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I108" s="1">
-        <v>0.47886403137853406</v>
+        <v>52.113596862146608</v>
       </c>
       <c r="J108" s="1">
-        <v>0.20921121576979412</v>
+        <v>79.078878423020583</v>
       </c>
       <c r="K108" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
@@ -4199,34 +4199,34 @@
         <v>2000</v>
       </c>
       <c r="B109" s="1">
-        <v>8.9974864308906596E-2</v>
+        <v>91.00251356910934</v>
       </c>
       <c r="C109" s="1">
-        <v>0.24490805676197291</v>
+        <v>75.509194323802703</v>
       </c>
       <c r="D109" s="1">
-        <v>1.326187706664925E-2</v>
+        <v>98.673812293335089</v>
       </c>
       <c r="E109" s="1">
-        <v>0.89566110948802302</v>
+        <v>10.43388905119769</v>
       </c>
       <c r="F109" s="1">
-        <v>0.65035938668803606</v>
+        <v>34.964061331196397</v>
       </c>
       <c r="G109" s="1">
-        <v>0.20945537809937767</v>
+        <v>79.054462190062239</v>
       </c>
       <c r="H109" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I109" s="1">
-        <v>0.48696029396764856</v>
+        <v>51.303970603235136</v>
       </c>
       <c r="J109" s="1">
-        <v>0.20743882572761871</v>
+        <v>79.256117427238109</v>
       </c>
       <c r="K109" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.2">
@@ -4234,34 +4234,34 @@
         <v>2001</v>
       </c>
       <c r="B110" s="1">
-        <v>9.2794549926860023E-2</v>
+        <v>90.720545007314001</v>
       </c>
       <c r="C110" s="1">
-        <v>0.23642772835206857</v>
+        <v>76.357227164793144</v>
       </c>
       <c r="D110" s="1">
-        <v>1.0492793105791289E-2</v>
+        <v>98.950720689420862</v>
       </c>
       <c r="E110" s="1">
-        <v>0.90319901606628594</v>
+        <v>9.6800983933714075</v>
       </c>
       <c r="F110" s="1">
-        <v>0.63667967125623537</v>
+        <v>36.332032874376473</v>
       </c>
       <c r="G110" s="1">
-        <v>0.24148828901412664</v>
+        <v>75.851171098587344</v>
       </c>
       <c r="H110" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I110" s="1">
-        <v>0.533368708843593</v>
+        <v>46.663129115640693</v>
       </c>
       <c r="J110" s="1">
-        <v>0.19914514157312094</v>
+        <v>80.085485842687902</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
@@ -4269,34 +4269,34 @@
         <v>2002</v>
       </c>
       <c r="B111" s="1">
-        <v>9.658763226941304E-2</v>
+        <v>90.341236773058711</v>
       </c>
       <c r="C111" s="1">
-        <v>0.24023534615416015</v>
+        <v>75.976465384583975</v>
       </c>
       <c r="D111" s="1">
-        <v>1.7090884165751039E-2</v>
+        <v>98.290911583424887</v>
       </c>
       <c r="E111" s="1">
-        <v>0.90956258752458963</v>
+        <v>9.0437412475410408</v>
       </c>
       <c r="F111" s="1">
-        <v>0.63044422246348897</v>
+        <v>36.955577753651106</v>
       </c>
       <c r="G111" s="1">
-        <v>0.24984606416696414</v>
+        <v>75.015393583303577</v>
       </c>
       <c r="H111" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I111" s="1">
-        <v>0.55245145361873527</v>
+        <v>44.754854638126481</v>
       </c>
       <c r="J111" s="1">
-        <v>0.22239324108985403</v>
+        <v>77.7606758910146</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
@@ -4304,34 +4304,34 @@
         <v>2003</v>
       </c>
       <c r="B112" s="1">
-        <v>9.1884326787151319E-2</v>
+        <v>90.811567321284855</v>
       </c>
       <c r="C112" s="1">
-        <v>0.23882600791407155</v>
+        <v>76.117399208592843</v>
       </c>
       <c r="D112" s="1">
-        <v>1.208056830472121E-2</v>
+        <v>98.791943169527883</v>
       </c>
       <c r="E112" s="1">
-        <v>0.91077289063158806</v>
+        <v>8.9227109368412023</v>
       </c>
       <c r="F112" s="1">
-        <v>0.62473478225248402</v>
+        <v>37.526521774751586</v>
       </c>
       <c r="G112" s="1">
-        <v>0.25397048623498775</v>
+        <v>74.602951376501224</v>
       </c>
       <c r="H112" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I112" s="1">
-        <v>0.56090067974162106</v>
+        <v>43.909932025837882</v>
       </c>
       <c r="J112" s="1">
-        <v>0.22620383401521912</v>
+        <v>77.37961659847808</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.2">
@@ -4339,34 +4339,34 @@
         <v>2004</v>
       </c>
       <c r="B113" s="1">
-        <v>9.3332435023556412E-2</v>
+        <v>90.666756497644357</v>
       </c>
       <c r="C113" s="1">
-        <v>0.25173727305014504</v>
+        <v>74.826272694985491</v>
       </c>
       <c r="D113" s="1">
-        <v>1.342165534989085E-2</v>
+        <v>98.657834465010922</v>
       </c>
       <c r="E113" s="1">
-        <v>0.91509850681692095</v>
+        <v>8.4901493183078998</v>
       </c>
       <c r="F113" s="1">
-        <v>0.62048631246058916</v>
+        <v>37.951368753941082</v>
       </c>
       <c r="G113" s="1">
-        <v>0.19945300717651526</v>
+        <v>80.05469928234848</v>
       </c>
       <c r="H113" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I113" s="1">
-        <v>0.56110356613951218</v>
+        <v>43.889643386048796</v>
       </c>
       <c r="J113" s="1">
-        <v>0.21975997871735653</v>
+        <v>78.024002128264343</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
@@ -4374,34 +4374,34 @@
         <v>2005</v>
       </c>
       <c r="B114" s="1">
-        <v>9.3660811776561825E-2</v>
+        <v>90.633918822343816</v>
       </c>
       <c r="C114" s="1">
-        <v>0.24482230125474952</v>
+        <v>75.517769874525044</v>
       </c>
       <c r="D114" s="1">
-        <v>1.3682873079808353E-2</v>
+        <v>98.631712692019164</v>
       </c>
       <c r="E114" s="1">
-        <v>0.92479354055913554</v>
+        <v>7.5206459440864419</v>
       </c>
       <c r="F114" s="1">
-        <v>0.61546605399894727</v>
+        <v>38.453394600105277</v>
       </c>
       <c r="G114" s="1">
-        <v>0.22436930747983636</v>
+        <v>77.563069252016376</v>
       </c>
       <c r="H114" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I114" s="1">
-        <v>0.52642585399114217</v>
+        <v>47.357414600885782</v>
       </c>
       <c r="J114" s="1">
-        <v>0.22027257548646853</v>
+        <v>77.972742451353156</v>
       </c>
       <c r="K114" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
@@ -4409,34 +4409,34 @@
         <v>2006</v>
       </c>
       <c r="B115" s="1">
-        <v>9.1039191066484559E-2</v>
+        <v>90.896080893351552</v>
       </c>
       <c r="C115" s="1">
-        <v>0.2626368931948676</v>
+        <v>73.736310680513242</v>
       </c>
       <c r="D115" s="1">
-        <v>1.5164169482674957E-2</v>
+        <v>98.483583051732509</v>
       </c>
       <c r="E115" s="1">
-        <v>0.9254080626575022</v>
+        <v>7.4591937342497801</v>
       </c>
       <c r="F115" s="1">
-        <v>0.61730512078655908</v>
+        <v>38.269487921344094</v>
       </c>
       <c r="G115" s="1">
-        <v>0.28381285938676365</v>
+        <v>71.618714061323644</v>
       </c>
       <c r="H115" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I115" s="1">
-        <v>0.5166801786080415</v>
+        <v>48.331982139195844</v>
       </c>
       <c r="J115" s="1">
-        <v>0.2227029484165704</v>
+        <v>77.729705158342966</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
@@ -4444,34 +4444,34 @@
         <v>2007</v>
       </c>
       <c r="B116" s="1">
-        <v>8.9403864582664666E-2</v>
+        <v>91.059613541733526</v>
       </c>
       <c r="C116" s="1">
-        <v>0.26932675007624574</v>
+        <v>73.067324992375433</v>
       </c>
       <c r="D116" s="1">
-        <v>1.1332044928818313E-2</v>
+        <v>98.866795507118169</v>
       </c>
       <c r="E116" s="1">
-        <v>0.92402936254713075</v>
+        <v>7.5970637452869179</v>
       </c>
       <c r="F116" s="1">
-        <v>0.61594670901998294</v>
+        <v>38.405329098001708</v>
       </c>
       <c r="G116" s="1">
-        <v>0.21375693143948377</v>
+        <v>78.624306856051632</v>
       </c>
       <c r="H116" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I116" s="1">
-        <v>0.52437249165145905</v>
+        <v>47.562750834854093</v>
       </c>
       <c r="J116" s="1">
-        <v>0.21538913865752329</v>
+        <v>78.461086134247665</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
@@ -4479,34 +4479,34 @@
         <v>2008</v>
       </c>
       <c r="B117" s="1">
-        <v>8.9327070477088238E-2</v>
+        <v>91.067292952291183</v>
       </c>
       <c r="C117" s="1">
-        <v>0.27119257937870095</v>
+        <v>72.880742062129912</v>
       </c>
       <c r="D117" s="1">
-        <v>1.6415085726836681E-2</v>
+        <v>98.358491427316324</v>
       </c>
       <c r="E117" s="1">
-        <v>0.92109391089796799</v>
+        <v>7.8906089102032064</v>
       </c>
       <c r="F117" s="1">
-        <v>0.61493059512217718</v>
+        <v>38.506940487782288</v>
       </c>
       <c r="G117" s="1">
-        <v>0.17218632043424384</v>
+        <v>82.781367956575608</v>
       </c>
       <c r="H117" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I117" s="1">
-        <v>0.55951779678104807</v>
+        <v>44.048220321895201</v>
       </c>
       <c r="J117" s="1">
-        <v>0.19620144580966553</v>
+        <v>80.379855419033447</v>
       </c>
       <c r="K117" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
@@ -4514,34 +4514,34 @@
         <v>2009</v>
       </c>
       <c r="B118" s="1">
-        <v>9.1190594489666377E-2</v>
+        <v>90.880940551033362</v>
       </c>
       <c r="C118" s="1">
-        <v>0.27588288163998986</v>
+        <v>72.411711836001018</v>
       </c>
       <c r="D118" s="1">
-        <v>1.5493512006842486E-2</v>
+        <v>98.450648799315758</v>
       </c>
       <c r="E118" s="1">
-        <v>0.9157380833101636</v>
+        <v>8.4261916689836358</v>
       </c>
       <c r="F118" s="1">
-        <v>0.61078443971005147</v>
+        <v>38.92155602899485</v>
       </c>
       <c r="G118" s="1">
-        <v>0.17319857137801492</v>
+        <v>82.680142862198508</v>
       </c>
       <c r="H118" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I118" s="1">
-        <v>0.5560345174435356</v>
+        <v>44.396548255646429</v>
       </c>
       <c r="J118" s="1">
-        <v>0.1927765142219969</v>
+        <v>80.722348577800304</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.2">
@@ -4549,34 +4549,34 @@
         <v>2010</v>
       </c>
       <c r="B119" s="1">
-        <v>9.0708695885717242E-2</v>
+        <v>90.929130411428289</v>
       </c>
       <c r="C119" s="1">
-        <v>0.27929296732872094</v>
+        <v>72.070703267127911</v>
       </c>
       <c r="D119" s="1">
-        <v>1.0630465316611413E-2</v>
+        <v>98.936953468338857</v>
       </c>
       <c r="E119" s="1">
-        <v>0.9097373772756151</v>
+        <v>9.0262622724384887</v>
       </c>
       <c r="F119" s="1">
-        <v>0.63784884457199731</v>
+        <v>36.21511554280027</v>
       </c>
       <c r="G119" s="1">
-        <v>0.20364973458642957</v>
+        <v>79.63502654135705</v>
       </c>
       <c r="H119" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I119" s="1">
-        <v>0.5753272735677567</v>
+        <v>42.467272643224319</v>
       </c>
       <c r="J119" s="1">
-        <v>0.23851347074854976</v>
+        <v>76.148652925145015</v>
       </c>
       <c r="K119" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
@@ -4584,34 +4584,34 @@
         <v>2011</v>
       </c>
       <c r="B120" s="1">
-        <v>8.8534378988803786E-2</v>
+        <v>91.146562101119628</v>
       </c>
       <c r="C120" s="1">
-        <v>0.27966275393867507</v>
+        <v>72.033724606132495</v>
       </c>
       <c r="D120" s="1">
-        <v>1.3349932424501065E-2</v>
+        <v>98.665006757549904</v>
       </c>
       <c r="E120" s="1">
-        <v>0.90774627534257657</v>
+        <v>9.2253724657423302</v>
       </c>
       <c r="F120" s="1">
-        <v>0.63679863857109131</v>
+        <v>36.320136142890867</v>
       </c>
       <c r="G120" s="1">
-        <v>0.20626965866062785</v>
+        <v>79.37303413393721</v>
       </c>
       <c r="H120" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I120" s="1">
-        <v>0.59161555187023507</v>
+        <v>40.838444812976505</v>
       </c>
       <c r="J120" s="1">
-        <v>0.24468632982536251</v>
+        <v>75.531367017463751</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
@@ -4619,34 +4619,34 @@
         <v>2012</v>
       </c>
       <c r="B121" s="1">
-        <v>9.1295852046312354E-2</v>
+        <v>90.870414795368774</v>
       </c>
       <c r="C121" s="1">
-        <v>0.2841243115784281</v>
+        <v>71.587568842157197</v>
       </c>
       <c r="D121" s="1">
-        <v>1.4881818200444945E-2</v>
+        <v>98.511818179955512</v>
       </c>
       <c r="E121" s="1">
-        <v>0.90730858802019843</v>
+        <v>9.2691411979801615</v>
       </c>
       <c r="F121" s="1">
-        <v>0.63966657332096377</v>
+        <v>36.033342667903632</v>
       </c>
       <c r="G121" s="1">
-        <v>0.20945406029982483</v>
+        <v>79.054593970017521</v>
       </c>
       <c r="H121" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I121" s="1">
-        <v>0.57191527901703665</v>
+        <v>42.808472098296342</v>
       </c>
       <c r="J121" s="1">
-        <v>0.2379341929626011</v>
+        <v>76.206580703739888</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
@@ -4654,34 +4654,34 @@
         <v>2013</v>
       </c>
       <c r="B122" s="1">
-        <v>9.4484012967354633E-2</v>
+        <v>90.551598703264531</v>
       </c>
       <c r="C122" s="1">
-        <v>0.29182081206420946</v>
+        <v>70.817918793579054</v>
       </c>
       <c r="D122" s="1">
-        <v>1.2472458489215195E-2</v>
+        <v>98.752754151078477</v>
       </c>
       <c r="E122" s="1">
-        <v>0.91049532828042146</v>
+        <v>8.9504671719578592</v>
       </c>
       <c r="F122" s="1">
-        <v>0.63935688979176808</v>
+        <v>36.064311020823176</v>
       </c>
       <c r="G122" s="1">
-        <v>0.15661404612325966</v>
+        <v>84.338595387674033</v>
       </c>
       <c r="H122" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I122" s="1">
-        <v>0.57739744371982527</v>
+        <v>42.260255628017475</v>
       </c>
       <c r="J122" s="1">
-        <v>0.25978499987068171</v>
+        <v>74.021500012931838</v>
       </c>
       <c r="K122" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.2">
@@ -4689,34 +4689,34 @@
         <v>2014</v>
       </c>
       <c r="B123" s="1">
-        <v>9.5143781930063662E-2</v>
+        <v>90.485621806993649</v>
       </c>
       <c r="C123" s="1">
-        <v>0.29624090197082348</v>
+        <v>70.375909802917661</v>
       </c>
       <c r="D123" s="1">
-        <v>1.2502663159495761E-2</v>
+        <v>98.749733684050412</v>
       </c>
       <c r="E123" s="1">
-        <v>0.91193607494752249</v>
+        <v>8.806392505247759</v>
       </c>
       <c r="F123" s="1">
-        <v>0.63660466709078989</v>
+        <v>36.339533290921004</v>
       </c>
       <c r="G123" s="1">
-        <v>0.16796710929080574</v>
+        <v>83.203289070919425</v>
       </c>
       <c r="H123" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I123" s="1">
-        <v>0.57447185602493955</v>
+        <v>42.55281439750604</v>
       </c>
       <c r="J123" s="1">
-        <v>0.25799909578870089</v>
+        <v>74.2000904211299</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
@@ -4724,34 +4724,34 @@
         <v>2015</v>
       </c>
       <c r="B124" s="1">
-        <v>9.6058117583686264E-2</v>
+        <v>90.394188241631369</v>
       </c>
       <c r="C124" s="1">
-        <v>0.29712056608534804</v>
+        <v>70.287943391465191</v>
       </c>
       <c r="D124" s="1">
-        <v>1.3225174482661105E-2</v>
+        <v>98.677482551733888</v>
       </c>
       <c r="E124" s="1">
-        <v>0.91158945286442139</v>
+        <v>8.8410547135578685</v>
       </c>
       <c r="F124" s="1">
-        <v>0.63403477483457815</v>
+        <v>36.596522516542187</v>
       </c>
       <c r="G124" s="1">
-        <v>0.17948846881633815</v>
+        <v>82.051153118366187</v>
       </c>
       <c r="H124" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I124" s="1">
-        <v>0.5706508792152668</v>
+        <v>42.934912078473317</v>
       </c>
       <c r="J124" s="1">
-        <v>0.26043486416220013</v>
+        <v>73.956513583779994</v>
       </c>
       <c r="K124" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.2">
@@ -4759,34 +4759,34 @@
         <v>1975</v>
       </c>
       <c r="B125" s="1">
-        <v>0.94168832559737492</v>
+        <v>5.8311674402625124</v>
       </c>
       <c r="C125" s="1">
-        <v>0.70812277416364444</v>
+        <v>29.187722583635555</v>
       </c>
       <c r="D125" s="1">
-        <v>0.98545279350712944</v>
+        <v>1.4547206492870601</v>
       </c>
       <c r="E125" s="1">
-        <v>0.1267781903718756</v>
+        <v>87.322180962812439</v>
       </c>
       <c r="F125" s="1">
-        <v>0.14718342581908037</v>
+        <v>85.281657418091967</v>
       </c>
       <c r="G125" s="1">
-        <v>0.70219778414744449</v>
+        <v>29.780221585255546</v>
       </c>
       <c r="H125" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I125" s="1">
-        <v>0.78985665339175737</v>
+        <v>21.014334660824264</v>
       </c>
       <c r="J125" s="1">
-        <v>0.63042845619866772</v>
+        <v>36.957154380133233</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
@@ -4794,34 +4794,34 @@
         <v>1976</v>
       </c>
       <c r="B126" s="1">
-        <v>0.94028592132328737</v>
+        <v>5.9714078676712532</v>
       </c>
       <c r="C126" s="1">
-        <v>0.72999976743143857</v>
+        <v>27.000023256856142</v>
       </c>
       <c r="D126" s="1">
-        <v>0.98575038611109145</v>
+        <v>1.4249613888908461</v>
       </c>
       <c r="E126" s="1">
-        <v>0.12895557026225249</v>
+        <v>87.104442973774738</v>
       </c>
       <c r="F126" s="1">
-        <v>0.17995136399351605</v>
+        <v>82.004863600648392</v>
       </c>
       <c r="G126" s="1">
-        <v>0.67445538571511132</v>
+        <v>32.554461428488857</v>
       </c>
       <c r="H126" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I126" s="1">
-        <v>0.82863222294243466</v>
+        <v>17.136777705756526</v>
       </c>
       <c r="J126" s="1">
-        <v>0.66616691972632847</v>
+        <v>33.383308027367143</v>
       </c>
       <c r="K126" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
@@ -4829,34 +4829,34 @@
         <v>1977</v>
       </c>
       <c r="B127" s="1">
-        <v>0.93815273480988826</v>
+        <v>6.1847265190111802</v>
       </c>
       <c r="C127" s="1">
-        <v>0.74520818974732894</v>
+        <v>25.479181025267117</v>
       </c>
       <c r="D127" s="1">
-        <v>0.98586198222067623</v>
+        <v>1.4138017779323921</v>
       </c>
       <c r="E127" s="1">
-        <v>0.12665343010926552</v>
+        <v>87.334656989073451</v>
       </c>
       <c r="F127" s="1">
-        <v>0.20310508243830888</v>
+        <v>79.689491756169119</v>
       </c>
       <c r="G127" s="1">
-        <v>0.68372419048039867</v>
+        <v>31.62758095196012</v>
       </c>
       <c r="H127" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I127" s="1">
-        <v>0.77916494171710116</v>
+        <v>22.083505828289887</v>
       </c>
       <c r="J127" s="1">
-        <v>0.68328297761893153</v>
+        <v>31.671702238106853</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.2">
@@ -4864,34 +4864,34 @@
         <v>1978</v>
       </c>
       <c r="B128" s="1">
-        <v>0.92954642994162551</v>
+        <v>7.0453570058374453</v>
       </c>
       <c r="C128" s="1">
-        <v>0.73845604295919653</v>
+        <v>26.154395704080347</v>
       </c>
       <c r="D128" s="1">
-        <v>0.98506286516560126</v>
+        <v>1.4937134834398669</v>
       </c>
       <c r="E128" s="1">
-        <v>0.13503931225559904</v>
+        <v>86.49606877444009</v>
       </c>
       <c r="F128" s="1">
-        <v>0.22687071629570912</v>
+        <v>77.312928370429077</v>
       </c>
       <c r="G128" s="1">
-        <v>0.67660722795680062</v>
+        <v>32.339277204319934</v>
       </c>
       <c r="H128" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I128" s="1">
-        <v>0.7881596298337612</v>
+        <v>21.184037016623886</v>
       </c>
       <c r="J128" s="1">
-        <v>0.734437570375578</v>
+        <v>26.556242962442202</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.2">
@@ -4899,34 +4899,34 @@
         <v>1979</v>
       </c>
       <c r="B129" s="1">
-        <v>0.92278562314616619</v>
+        <v>7.7214376853833793</v>
       </c>
       <c r="C129" s="1">
-        <v>0.72817045528810542</v>
+        <v>27.182954471189458</v>
       </c>
       <c r="D129" s="1">
-        <v>0.98160083501131279</v>
+        <v>1.8399164988687149</v>
       </c>
       <c r="E129" s="1">
-        <v>0.14835351803076788</v>
+        <v>85.164648196923224</v>
       </c>
       <c r="F129" s="1">
-        <v>0.23299964852078975</v>
+        <v>76.700035147921028</v>
       </c>
       <c r="G129" s="1">
-        <v>0.75545587085258248</v>
+        <v>24.454412914741749</v>
       </c>
       <c r="H129" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I129" s="1">
-        <v>0.77845246495701326</v>
+        <v>22.154753504298668</v>
       </c>
       <c r="J129" s="1">
-        <v>0.75281337216581257</v>
+        <v>24.71866278341875</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.2">
@@ -4934,34 +4934,34 @@
         <v>1980</v>
       </c>
       <c r="B130" s="1">
-        <v>0.91973622346088613</v>
+        <v>8.0263776539113874</v>
       </c>
       <c r="C130" s="1">
-        <v>0.71721813240387322</v>
+        <v>28.278186759612687</v>
       </c>
       <c r="D130" s="1">
-        <v>0.98432460756226492</v>
+        <v>1.5675392437735123</v>
       </c>
       <c r="E130" s="1">
-        <v>0.16229632573249689</v>
+        <v>83.770367426750298</v>
       </c>
       <c r="F130" s="1">
-        <v>0.24673563230480278</v>
+        <v>75.326436769519717</v>
       </c>
       <c r="G130" s="1">
-        <v>0.64123205050723897</v>
+        <v>35.876794949276103</v>
       </c>
       <c r="H130" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I130" s="1">
-        <v>0.77141224760494742</v>
+        <v>22.858775239505263</v>
       </c>
       <c r="J130" s="1">
-        <v>0.76516518592218519</v>
+        <v>23.483481407781483</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.2">
@@ -4969,34 +4969,34 @@
         <v>1981</v>
       </c>
       <c r="B131" s="1">
-        <v>0.91810452777487883</v>
+        <v>8.1895472225121182</v>
       </c>
       <c r="C131" s="1">
-        <v>0.7428271748516444</v>
+        <v>25.71728251483556</v>
       </c>
       <c r="D131" s="1">
-        <v>0.98700017955035879</v>
+        <v>1.2999820449641148</v>
       </c>
       <c r="E131" s="1">
-        <v>0.18403958337277496</v>
+        <v>81.596041662722513</v>
       </c>
       <c r="F131" s="1">
-        <v>0.24307467043261563</v>
+        <v>75.692532956738432</v>
       </c>
       <c r="G131" s="1">
-        <v>0.65866813317290529</v>
+        <v>34.133186682709471</v>
       </c>
       <c r="H131" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I131" s="1">
-        <v>0.70470189868767719</v>
+        <v>29.529810131232271</v>
       </c>
       <c r="J131" s="1">
-        <v>0.80321106815429921</v>
+        <v>19.678893184570075</v>
       </c>
       <c r="K131" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.2">
@@ -5004,34 +5004,34 @@
         <v>1982</v>
       </c>
       <c r="B132" s="1">
-        <v>0.91668427808838504</v>
+        <v>8.3315721911614951</v>
       </c>
       <c r="C132" s="1">
-        <v>0.74786337482999654</v>
+        <v>25.213662517000351</v>
       </c>
       <c r="D132" s="1">
-        <v>0.98469504545087261</v>
+        <v>1.5304954549127396</v>
       </c>
       <c r="E132" s="1">
-        <v>0.16585560994663587</v>
+        <v>83.414439005336405</v>
       </c>
       <c r="F132" s="1">
-        <v>0.25902573343033364</v>
+        <v>74.097426656966633</v>
       </c>
       <c r="G132" s="1">
-        <v>0.64932118107445169</v>
+        <v>35.067881892554844</v>
       </c>
       <c r="H132" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I132" s="1">
-        <v>0.7884739656546158</v>
+        <v>21.152603434538431</v>
       </c>
       <c r="J132" s="1">
-        <v>0.81629408551973848</v>
+        <v>18.370591448026154</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.2">
@@ -5039,34 +5039,34 @@
         <v>1983</v>
       </c>
       <c r="B133" s="1">
-        <v>0.91378082401894689</v>
+        <v>8.6219175981053198</v>
       </c>
       <c r="C133" s="1">
-        <v>0.74684568281178387</v>
+        <v>25.315431718821618</v>
       </c>
       <c r="D133" s="1">
-        <v>0.98428732618863624</v>
+        <v>1.571267381136374</v>
       </c>
       <c r="E133" s="1">
-        <v>0.15819469098213479</v>
+        <v>84.180530901786526</v>
       </c>
       <c r="F133" s="1">
-        <v>0.276793427327574</v>
+        <v>72.320657267242595</v>
       </c>
       <c r="G133" s="1">
-        <v>0.74149904041354375</v>
+        <v>25.850095958645618</v>
       </c>
       <c r="H133" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I133" s="1">
-        <v>0.77383219053706043</v>
+        <v>22.616780946293961</v>
       </c>
       <c r="J133" s="1">
-        <v>0.82663621224767481</v>
+        <v>17.336378775232532</v>
       </c>
       <c r="K133" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.2">
@@ -5074,34 +5074,34 @@
         <v>1984</v>
       </c>
       <c r="B134" s="1">
-        <v>0.90820849064545039</v>
+        <v>9.1791509354549525</v>
       </c>
       <c r="C134" s="1">
-        <v>0.74657795557602713</v>
+        <v>25.342204442397286</v>
       </c>
       <c r="D134" s="1">
-        <v>0.98529205785700735</v>
+        <v>1.4707942142992714</v>
       </c>
       <c r="E134" s="1">
-        <v>0.15348789171145882</v>
+        <v>84.651210828854119</v>
       </c>
       <c r="F134" s="1">
-        <v>0.28448825158327801</v>
+        <v>71.551174841672207</v>
       </c>
       <c r="G134" s="1">
-        <v>0.75782783828495426</v>
+        <v>24.217216171504582</v>
       </c>
       <c r="H134" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I134" s="1">
-        <v>0.72117780262176734</v>
+        <v>27.882219737823267</v>
       </c>
       <c r="J134" s="1">
-        <v>0.83070215478585041</v>
+        <v>16.929784521414952</v>
       </c>
       <c r="K134" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.2">
@@ -5109,34 +5109,34 @@
         <v>1985</v>
       </c>
       <c r="B135" s="1">
-        <v>0.90636342117232249</v>
+        <v>9.363657882767761</v>
       </c>
       <c r="C135" s="1">
-        <v>0.74684475520235416</v>
+        <v>25.315524479764591</v>
       </c>
       <c r="D135" s="1">
-        <v>0.98617062950972556</v>
+        <v>1.3829370490274351</v>
       </c>
       <c r="E135" s="1">
-        <v>0.15011736237589715</v>
+        <v>84.988263762410284</v>
       </c>
       <c r="F135" s="1">
-        <v>0.29421895173682888</v>
+        <v>70.578104826317116</v>
       </c>
       <c r="G135" s="1">
-        <v>0.74905766437955834</v>
+        <v>25.094233562044167</v>
       </c>
       <c r="H135" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I135" s="1">
-        <v>0.72129424470563885</v>
+        <v>27.87057552943612</v>
       </c>
       <c r="J135" s="1">
-        <v>0.8376827464544857</v>
+        <v>16.231725354551426</v>
       </c>
       <c r="K135" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.2">
@@ -5144,34 +5144,34 @@
         <v>1986</v>
       </c>
       <c r="B136" s="1">
-        <v>0.90360612953650332</v>
+        <v>9.6393870463496629</v>
       </c>
       <c r="C136" s="1">
-        <v>0.72967409204452305</v>
+        <v>27.032590795547684</v>
       </c>
       <c r="D136" s="1">
-        <v>0.9884764751210191</v>
+        <v>1.1523524878980884</v>
       </c>
       <c r="E136" s="1">
-        <v>0.15338248746158586</v>
+        <v>84.661751253841416</v>
       </c>
       <c r="F136" s="1">
-        <v>0.29866072572315772</v>
+        <v>70.133927427684213</v>
       </c>
       <c r="G136" s="1">
-        <v>0.75025439281733874</v>
+        <v>24.974560718266122</v>
       </c>
       <c r="H136" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I136" s="1">
-        <v>0.71241068663151874</v>
+        <v>28.758931336848125</v>
       </c>
       <c r="J136" s="1">
-        <v>0.84165063701251908</v>
+        <v>15.83493629874809</v>
       </c>
       <c r="K136" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.2">
@@ -5179,34 +5179,34 @@
         <v>1987</v>
       </c>
       <c r="B137" s="1">
-        <v>0.90518313913686432</v>
+        <v>9.4816860863135712</v>
       </c>
       <c r="C137" s="1">
-        <v>0.72348578377860739</v>
+        <v>27.651421622139267</v>
       </c>
       <c r="D137" s="1">
-        <v>0.98956550814267741</v>
+        <v>1.0434491857322576</v>
       </c>
       <c r="E137" s="1">
-        <v>0.14651974587888644</v>
+        <v>85.348025412111355</v>
       </c>
       <c r="F137" s="1">
-        <v>0.30371242878261373</v>
+        <v>69.62875712173863</v>
       </c>
       <c r="G137" s="1">
-        <v>0.74316844080089506</v>
+        <v>25.683155919910494</v>
       </c>
       <c r="H137" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I137" s="1">
-        <v>0.73546853684574687</v>
+        <v>26.453146315425315</v>
       </c>
       <c r="J137" s="1">
-        <v>0.83607298006017927</v>
+        <v>16.392701993982072</v>
       </c>
       <c r="K137" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.2">
@@ -5214,34 +5214,34 @@
         <v>1988</v>
       </c>
       <c r="B138" s="1">
-        <v>0.90671069357334111</v>
+        <v>9.3289306426658811</v>
       </c>
       <c r="C138" s="1">
-        <v>0.73191391989613741</v>
+        <v>26.808608010386255</v>
       </c>
       <c r="D138" s="1">
-        <v>0.98997879284181345</v>
+        <v>1.0021207158186565</v>
       </c>
       <c r="E138" s="1">
-        <v>0.14612196059799823</v>
+        <v>85.387803940200186</v>
       </c>
       <c r="F138" s="1">
-        <v>0.30838564661245293</v>
+        <v>69.1614353387547</v>
       </c>
       <c r="G138" s="1">
-        <v>0.81542304792783171</v>
+        <v>18.457695207216826</v>
       </c>
       <c r="H138" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I138" s="1">
-        <v>0.65216962082756846</v>
+        <v>34.783037917243156</v>
       </c>
       <c r="J138" s="1">
-        <v>0.83339426586180221</v>
+        <v>16.660573413819773</v>
       </c>
       <c r="K138" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.2">
@@ -5249,34 +5249,34 @@
         <v>1989</v>
       </c>
       <c r="B139" s="1">
-        <v>0.91014206334438863</v>
+        <v>8.9857936655611308</v>
       </c>
       <c r="C139" s="1">
-        <v>0.7446630004122915</v>
+        <v>25.53369995877085</v>
       </c>
       <c r="D139" s="1">
-        <v>0.9901292989364272</v>
+        <v>0.98707010635727122</v>
       </c>
       <c r="E139" s="1">
-        <v>0.15065660080197785</v>
+        <v>84.934339919802198</v>
       </c>
       <c r="F139" s="1">
-        <v>0.3159182144331536</v>
+        <v>68.408178556684646</v>
       </c>
       <c r="G139" s="1">
-        <v>0.81345833269489898</v>
+        <v>18.654166730510109</v>
       </c>
       <c r="H139" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I139" s="1">
-        <v>0.56708718310888384</v>
+        <v>43.291281689111607</v>
       </c>
       <c r="J139" s="1">
-        <v>0.83043086671913091</v>
+        <v>16.956913328086916</v>
       </c>
       <c r="K139" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.2">
@@ -5284,34 +5284,34 @@
         <v>1990</v>
       </c>
       <c r="B140" s="1">
-        <v>0.90160469454497405</v>
+        <v>9.839530545502603</v>
       </c>
       <c r="C140" s="1">
-        <v>0.7633303938183339</v>
+        <v>23.666960618166609</v>
       </c>
       <c r="D140" s="1">
-        <v>0.99042778552559152</v>
+        <v>0.95722144744084681</v>
       </c>
       <c r="E140" s="1">
-        <v>0.1522915199093865</v>
+        <v>84.770848009061353</v>
       </c>
       <c r="F140" s="1">
-        <v>0.32866744438010287</v>
+        <v>67.133255561989699</v>
       </c>
       <c r="G140" s="1">
-        <v>0.81947716934436499</v>
+        <v>18.052283065563497</v>
       </c>
       <c r="H140" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I140" s="1">
-        <v>0.60611537750847322</v>
+        <v>39.388462249152681</v>
       </c>
       <c r="J140" s="1">
-        <v>0.84360877263864975</v>
+        <v>15.639122736135016</v>
       </c>
       <c r="K140" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.2">
@@ -5319,34 +5319,34 @@
         <v>1991</v>
       </c>
       <c r="B141" s="1">
-        <v>0.89996181930706931</v>
+        <v>10.00381806929307</v>
       </c>
       <c r="C141" s="1">
-        <v>0.76844402743578188</v>
+        <v>23.155597256421807</v>
       </c>
       <c r="D141" s="1">
-        <v>0.9910022913153288</v>
+        <v>0.89977086846712451</v>
       </c>
       <c r="E141" s="1">
-        <v>0.15628511276971421</v>
+        <v>84.371488723028577</v>
       </c>
       <c r="F141" s="1">
-        <v>0.33811448413105272</v>
+        <v>66.188551586894732</v>
       </c>
       <c r="G141" s="1">
-        <v>0.83146476949298531</v>
+        <v>16.853523050701465</v>
       </c>
       <c r="H141" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I141" s="1">
-        <v>0.58276568277777718</v>
+        <v>41.723431722222273</v>
       </c>
       <c r="J141" s="1">
-        <v>0.85290665820184586</v>
+        <v>14.709334179815414</v>
       </c>
       <c r="K141" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.2">
@@ -5354,34 +5354,34 @@
         <v>1992</v>
       </c>
       <c r="B142" s="1">
-        <v>0.89925563204818171</v>
+        <v>10.074436795181827</v>
       </c>
       <c r="C142" s="1">
-        <v>0.76793371072363048</v>
+        <v>23.206628927636956</v>
       </c>
       <c r="D142" s="1">
-        <v>0.99092899805506929</v>
+        <v>0.90710019449306256</v>
       </c>
       <c r="E142" s="1">
-        <v>0.1528944813267204</v>
+        <v>84.710551867327951</v>
       </c>
       <c r="F142" s="1">
-        <v>0.34113927073267808</v>
+        <v>65.886072926732197</v>
       </c>
       <c r="G142" s="1">
-        <v>0.82356224512929443</v>
+        <v>17.643775487070563</v>
       </c>
       <c r="H142" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I142" s="1">
-        <v>0.56799105484244827</v>
+        <v>43.200894515755181</v>
       </c>
       <c r="J142" s="1">
-        <v>0.85081778638075689</v>
+        <v>14.918221361924303</v>
       </c>
       <c r="K142" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.2">
@@ -5389,34 +5389,34 @@
         <v>1993</v>
       </c>
       <c r="B143" s="1">
-        <v>0.89442149830324669</v>
+        <v>10.557850169675321</v>
       </c>
       <c r="C143" s="1">
-        <v>0.7546243657978442</v>
+        <v>24.537563420215591</v>
       </c>
       <c r="D143" s="1">
-        <v>0.99065139865673613</v>
+        <v>0.93486013432638837</v>
       </c>
       <c r="E143" s="1">
-        <v>0.14241851471488656</v>
+        <v>85.758148528511342</v>
       </c>
       <c r="F143" s="1">
-        <v>0.33146346179504221</v>
+        <v>66.853653820495779</v>
       </c>
       <c r="G143" s="1">
-        <v>0.81817796687475741</v>
+        <v>18.182203312524258</v>
       </c>
       <c r="H143" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I143" s="1">
-        <v>0.50287710432088906</v>
+        <v>49.712289567911085</v>
       </c>
       <c r="J143" s="1">
-        <v>0.8391943634415473</v>
+        <v>16.080563655845275</v>
       </c>
       <c r="K143" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.2">
@@ -5424,34 +5424,34 @@
         <v>1994</v>
       </c>
       <c r="B144" s="1">
-        <v>0.89253428445501493</v>
+        <v>10.7465715544985</v>
       </c>
       <c r="C144" s="1">
-        <v>0.74971132216889047</v>
+        <v>25.028867783110957</v>
       </c>
       <c r="D144" s="1">
-        <v>0.99039139832991041</v>
+        <v>0.96086016700896071</v>
       </c>
       <c r="E144" s="1">
-        <v>0.13154877814487045</v>
+        <v>86.845122185512963</v>
       </c>
       <c r="F144" s="1">
-        <v>0.32408889430491683</v>
+        <v>67.591110569508317</v>
       </c>
       <c r="G144" s="1">
-        <v>0.85496253867000083</v>
+        <v>14.503746132999918</v>
       </c>
       <c r="H144" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I144" s="1">
-        <v>0.48683855368025025</v>
+        <v>51.316144631974957</v>
       </c>
       <c r="J144" s="1">
-        <v>0.83791891311285038</v>
+        <v>16.208108688714955</v>
       </c>
       <c r="K144" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.2">
@@ -5459,34 +5459,34 @@
         <v>1995</v>
       </c>
       <c r="B145" s="1">
-        <v>0.90169782400263665</v>
+        <v>9.830217599736347</v>
       </c>
       <c r="C145" s="1">
-        <v>0.75465887502208706</v>
+        <v>24.534112497791302</v>
       </c>
       <c r="D145" s="1">
-        <v>0.98972563130782909</v>
+        <v>1.0274368692170914</v>
       </c>
       <c r="E145" s="1">
-        <v>0.12132562065759785</v>
+        <v>87.867437934240215</v>
       </c>
       <c r="F145" s="1">
-        <v>0.3303945622883423</v>
+        <v>66.960543771165788</v>
       </c>
       <c r="G145" s="1">
-        <v>0.80595661355800741</v>
+        <v>19.404338644199264</v>
       </c>
       <c r="H145" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I145" s="1">
-        <v>0.47938697018714554</v>
+        <v>52.061302981285451</v>
       </c>
       <c r="J145" s="1">
-        <v>0.82258032180078366</v>
+        <v>17.741967819921626</v>
       </c>
       <c r="K145" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.2">
@@ -5494,34 +5494,34 @@
         <v>1996</v>
       </c>
       <c r="B146" s="1">
-        <v>0.90727757952961807</v>
+        <v>9.272242047038187</v>
       </c>
       <c r="C146" s="1">
-        <v>0.75791092193578879</v>
+        <v>24.20890780642112</v>
       </c>
       <c r="D146" s="1">
-        <v>0.9889096283042178</v>
+        <v>1.10903716957821</v>
       </c>
       <c r="E146" s="1">
-        <v>0.11343139473130637</v>
+        <v>88.656860526869366</v>
       </c>
       <c r="F146" s="1">
-        <v>0.31874163857488091</v>
+        <v>68.125836142511915</v>
       </c>
       <c r="G146" s="1">
-        <v>0.78053738549013396</v>
+        <v>21.946261450986604</v>
       </c>
       <c r="H146" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I146" s="1">
-        <v>0.4686445965832442</v>
+        <v>53.135540341675593</v>
       </c>
       <c r="J146" s="1">
-        <v>0.82455570942245437</v>
+        <v>17.544429057754567</v>
       </c>
       <c r="K146" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.2">
@@ -5529,34 +5529,34 @@
         <v>1997</v>
       </c>
       <c r="B147" s="1">
-        <v>0.90551052314870883</v>
+        <v>9.4489476851291183</v>
       </c>
       <c r="C147" s="1">
-        <v>0.7622070750988551</v>
+        <v>23.779292490114482</v>
       </c>
       <c r="D147" s="1">
-        <v>0.98919162343440048</v>
+        <v>1.0808376565599611</v>
       </c>
       <c r="E147" s="1">
-        <v>0.10727809072460939</v>
+        <v>89.272190927539071</v>
       </c>
       <c r="F147" s="1">
-        <v>0.31269992147204656</v>
+        <v>68.730007852795339</v>
       </c>
       <c r="G147" s="1">
-        <v>0.82830499499504051</v>
+        <v>17.169500500495946</v>
       </c>
       <c r="H147" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I147" s="1">
-        <v>0.48516475507477497</v>
+        <v>51.483524492522506</v>
       </c>
       <c r="J147" s="1">
-        <v>0.82637968191917655</v>
+        <v>17.362031808082346</v>
       </c>
       <c r="K147" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.2">
@@ -5564,34 +5564,34 @@
         <v>1998</v>
       </c>
       <c r="B148" s="1">
-        <v>0.90970136664288836</v>
+        <v>9.0298633357111573</v>
       </c>
       <c r="C148" s="1">
-        <v>0.76442712447774086</v>
+        <v>23.557287552225915</v>
       </c>
       <c r="D148" s="1">
-        <v>0.98782614924145029</v>
+        <v>1.2173850758549662</v>
       </c>
       <c r="E148" s="1">
-        <v>0.10329939716501062</v>
+        <v>89.670060283498941</v>
       </c>
       <c r="F148" s="1">
-        <v>0.31749293672202394</v>
+        <v>68.250706327797616</v>
       </c>
       <c r="G148" s="1">
-        <v>0.81425051953345395</v>
+        <v>18.574948046654598</v>
       </c>
       <c r="H148" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I148" s="1">
-        <v>0.54761438647675742</v>
+        <v>45.238561352324261</v>
       </c>
       <c r="J148" s="1">
-        <v>0.80371391825999128</v>
+        <v>19.628608174000885</v>
       </c>
       <c r="K148" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.2">
@@ -5599,34 +5599,34 @@
         <v>1999</v>
       </c>
       <c r="B149" s="1">
-        <v>0.90903270908658629</v>
+        <v>9.0967290913413663</v>
       </c>
       <c r="C149" s="1">
-        <v>0.75979339142043556</v>
+        <v>24.020660857956432</v>
       </c>
       <c r="D149" s="1">
-        <v>0.98767269409341696</v>
+        <v>1.2327305906583139</v>
       </c>
       <c r="E149" s="1">
-        <v>0.10383205118782457</v>
+        <v>89.616794881217544</v>
       </c>
       <c r="F149" s="1">
-        <v>0.33467614142344221</v>
+        <v>66.532385857655783</v>
       </c>
       <c r="G149" s="1">
-        <v>0.74861194679260123</v>
+        <v>25.13880532073987</v>
       </c>
       <c r="H149" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I149" s="1">
-        <v>0.52113596862146605</v>
+        <v>47.886403137853407</v>
       </c>
       <c r="J149" s="1">
-        <v>0.79078878423020582</v>
+        <v>20.921121576979413</v>
       </c>
       <c r="K149" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.2">
@@ -5634,34 +5634,34 @@
         <v>2000</v>
       </c>
       <c r="B150" s="1">
-        <v>0.91002513569109345</v>
+        <v>8.9974864308906604</v>
       </c>
       <c r="C150" s="1">
-        <v>0.75509194323802697</v>
+        <v>24.49080567619729</v>
       </c>
       <c r="D150" s="1">
-        <v>0.98673812293335084</v>
+        <v>1.326187706664925</v>
       </c>
       <c r="E150" s="1">
-        <v>0.1043388905119769</v>
+        <v>89.566110948802304</v>
       </c>
       <c r="F150" s="1">
-        <v>0.349640613311964</v>
+        <v>65.03593866880361</v>
       </c>
       <c r="G150" s="1">
-        <v>0.79054462190062236</v>
+        <v>20.945537809937768</v>
       </c>
       <c r="H150" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I150" s="1">
-        <v>0.51303970603235138</v>
+        <v>48.696029396764857</v>
       </c>
       <c r="J150" s="1">
-        <v>0.79256117427238115</v>
+        <v>20.743882572761869</v>
       </c>
       <c r="K150" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.2">
@@ -5669,34 +5669,34 @@
         <v>2001</v>
       </c>
       <c r="B151" s="1">
-        <v>0.90720545007314002</v>
+        <v>9.2794549926860022</v>
       </c>
       <c r="C151" s="1">
-        <v>0.7635722716479314</v>
+        <v>23.642772835206856</v>
       </c>
       <c r="D151" s="1">
-        <v>0.98950720689420868</v>
+        <v>1.0492793105791289</v>
       </c>
       <c r="E151" s="1">
-        <v>9.6800983933714072E-2</v>
+        <v>90.319901606628591</v>
       </c>
       <c r="F151" s="1">
-        <v>0.36332032874376474</v>
+        <v>63.667967125623534</v>
       </c>
       <c r="G151" s="1">
-        <v>0.75851171098587344</v>
+        <v>24.148828901412664</v>
       </c>
       <c r="H151" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I151" s="1">
-        <v>0.46663129115640695</v>
+        <v>53.3368708843593</v>
       </c>
       <c r="J151" s="1">
-        <v>0.80085485842687898</v>
+        <v>19.914514157312095</v>
       </c>
       <c r="K151" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.2">
@@ -5704,34 +5704,34 @@
         <v>2002</v>
       </c>
       <c r="B152" s="1">
-        <v>0.90341236773058708</v>
+        <v>9.6587632269413035</v>
       </c>
       <c r="C152" s="1">
-        <v>0.7597646538458398</v>
+        <v>24.023534615416015</v>
       </c>
       <c r="D152" s="1">
-        <v>0.98290911583424889</v>
+        <v>1.7090884165751039</v>
       </c>
       <c r="E152" s="1">
-        <v>9.0437412475410414E-2</v>
+        <v>90.956258752458965</v>
       </c>
       <c r="F152" s="1">
-        <v>0.36955577753651103</v>
+        <v>63.044422246348894</v>
       </c>
       <c r="G152" s="1">
-        <v>0.7501539358330358</v>
+        <v>24.984606416696415</v>
       </c>
       <c r="H152" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I152" s="1">
-        <v>0.44754854638126479</v>
+        <v>55.245145361873526</v>
       </c>
       <c r="J152" s="1">
-        <v>0.77760675891014597</v>
+        <v>22.239324108985404</v>
       </c>
       <c r="K152" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.2">
@@ -5739,34 +5739,34 @@
         <v>2003</v>
       </c>
       <c r="B153" s="1">
-        <v>0.90811567321284858</v>
+        <v>9.1884326787151327</v>
       </c>
       <c r="C153" s="1">
-        <v>0.7611739920859284</v>
+        <v>23.882600791407153</v>
       </c>
       <c r="D153" s="1">
-        <v>0.98791943169527885</v>
+        <v>1.2080568304721211</v>
       </c>
       <c r="E153" s="1">
-        <v>8.9227109368412022E-2</v>
+        <v>91.077289063158801</v>
       </c>
       <c r="F153" s="1">
-        <v>0.37526521774751587</v>
+        <v>62.4734782252484</v>
       </c>
       <c r="G153" s="1">
-        <v>0.74602951376501225</v>
+        <v>25.397048623498776</v>
       </c>
       <c r="H153" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I153" s="1">
-        <v>0.43909932025837883</v>
+        <v>56.090067974162103</v>
       </c>
       <c r="J153" s="1">
-        <v>0.77379616598478085</v>
+        <v>22.620383401521913</v>
       </c>
       <c r="K153" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.2">
@@ -5774,34 +5774,34 @@
         <v>2004</v>
       </c>
       <c r="B154" s="1">
-        <v>0.90666756497644363</v>
+        <v>9.333243502355641</v>
       </c>
       <c r="C154" s="1">
-        <v>0.74826272694985496</v>
+        <v>25.173727305014502</v>
       </c>
       <c r="D154" s="1">
-        <v>0.98657834465010918</v>
+        <v>1.3421655349890851</v>
       </c>
       <c r="E154" s="1">
-        <v>8.4901493183079005E-2</v>
+        <v>91.5098506816921</v>
       </c>
       <c r="F154" s="1">
-        <v>0.37951368753941084</v>
+        <v>62.048631246058918</v>
       </c>
       <c r="G154" s="1">
-        <v>0.80054699282348474</v>
+        <v>19.945300717651527</v>
       </c>
       <c r="H154" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I154" s="1">
-        <v>0.43889643386048793</v>
+        <v>56.110356613951218</v>
       </c>
       <c r="J154" s="1">
-        <v>0.78024002128264336</v>
+        <v>21.975997871735654</v>
       </c>
       <c r="K154" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.2">
@@ -5809,34 +5809,34 @@
         <v>2005</v>
       </c>
       <c r="B155" s="1">
-        <v>0.90633918822343817</v>
+        <v>9.3660811776561825</v>
       </c>
       <c r="C155" s="1">
-        <v>0.75517769874525043</v>
+        <v>24.482230125474953</v>
       </c>
       <c r="D155" s="1">
-        <v>0.98631712692019169</v>
+        <v>1.3682873079808353</v>
       </c>
       <c r="E155" s="1">
-        <v>7.5206459440864418E-2</v>
+        <v>92.479354055913561</v>
       </c>
       <c r="F155" s="1">
-        <v>0.38453394600105278</v>
+        <v>61.54660539989473</v>
       </c>
       <c r="G155" s="1">
-        <v>0.7756306925201637</v>
+        <v>22.436930747983634</v>
       </c>
       <c r="H155" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I155" s="1">
-        <v>0.47357414600885783</v>
+        <v>52.642585399114218</v>
       </c>
       <c r="J155" s="1">
-        <v>0.7797274245135315</v>
+        <v>22.027257548646855</v>
       </c>
       <c r="K155" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.2">
@@ -5844,34 +5844,34 @@
         <v>2006</v>
       </c>
       <c r="B156" s="1">
-        <v>0.9089608089335155</v>
+        <v>9.1039191066484566</v>
       </c>
       <c r="C156" s="1">
-        <v>0.7373631068051324</v>
+        <v>26.263689319486762</v>
       </c>
       <c r="D156" s="1">
-        <v>0.98483583051732515</v>
+        <v>1.5164169482674956</v>
       </c>
       <c r="E156" s="1">
-        <v>7.4591937342497805E-2</v>
+        <v>92.54080626575022</v>
       </c>
       <c r="F156" s="1">
-        <v>0.38269487921344097</v>
+        <v>61.730512078655906</v>
       </c>
       <c r="G156" s="1">
-        <v>0.71618714061323641</v>
+        <v>28.381285938676363</v>
       </c>
       <c r="H156" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I156" s="1">
-        <v>0.48331982139195845</v>
+        <v>51.668017860804149</v>
       </c>
       <c r="J156" s="1">
-        <v>0.77729705158342965</v>
+        <v>22.270294841657041</v>
       </c>
       <c r="K156" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.2">
@@ -5879,34 +5879,34 @@
         <v>2007</v>
       </c>
       <c r="B157" s="1">
-        <v>0.91059613541733531</v>
+        <v>8.9403864582664667</v>
       </c>
       <c r="C157" s="1">
-        <v>0.73067324992375426</v>
+        <v>26.932675007624574</v>
       </c>
       <c r="D157" s="1">
-        <v>0.98866795507118166</v>
+        <v>1.1332044928818314</v>
       </c>
       <c r="E157" s="1">
-        <v>7.597063745286918E-2</v>
+        <v>92.402936254713069</v>
       </c>
       <c r="F157" s="1">
-        <v>0.38405329098001711</v>
+        <v>61.594670901998292</v>
       </c>
       <c r="G157" s="1">
-        <v>0.78624306856051629</v>
+        <v>21.375693143948375</v>
       </c>
       <c r="H157" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I157" s="1">
-        <v>0.47562750834854089</v>
+        <v>52.437249165145907</v>
       </c>
       <c r="J157" s="1">
-        <v>0.7846108613424766</v>
+        <v>21.538913865752328</v>
       </c>
       <c r="K157" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.2">
@@ -5914,34 +5914,34 @@
         <v>2008</v>
       </c>
       <c r="B158" s="1">
-        <v>0.91067292952291179</v>
+        <v>8.9327070477088242</v>
       </c>
       <c r="C158" s="1">
-        <v>0.72880742062129911</v>
+        <v>27.119257937870096</v>
       </c>
       <c r="D158" s="1">
-        <v>0.9835849142731633</v>
+        <v>1.641508572683668</v>
       </c>
       <c r="E158" s="1">
-        <v>7.8906089102032062E-2</v>
+        <v>92.109391089796802</v>
       </c>
       <c r="F158" s="1">
-        <v>0.38506940487782287</v>
+        <v>61.493059512217719</v>
       </c>
       <c r="G158" s="1">
-        <v>0.82781367956575613</v>
+        <v>17.218632043424385</v>
       </c>
       <c r="H158" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I158" s="1">
-        <v>0.44048220321895198</v>
+        <v>55.951779678104806</v>
       </c>
       <c r="J158" s="1">
-        <v>0.80379855419033441</v>
+        <v>19.620144580966553</v>
       </c>
       <c r="K158" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.2">
@@ -5949,34 +5949,34 @@
         <v>2009</v>
       </c>
       <c r="B159" s="1">
-        <v>0.90880940551033362</v>
+        <v>9.1190594489666381</v>
       </c>
       <c r="C159" s="1">
-        <v>0.72411711836001025</v>
+        <v>27.588288163998985</v>
       </c>
       <c r="D159" s="1">
-        <v>0.98450648799315754</v>
+        <v>1.5493512006842485</v>
       </c>
       <c r="E159" s="1">
-        <v>8.4261916689836361E-2</v>
+        <v>91.573808331016366</v>
       </c>
       <c r="F159" s="1">
-        <v>0.38921556028994853</v>
+        <v>61.07844397100515</v>
       </c>
       <c r="G159" s="1">
-        <v>0.82680142862198513</v>
+        <v>17.319857137801492</v>
       </c>
       <c r="H159" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I159" s="1">
-        <v>0.44396548255646429</v>
+        <v>55.603451744353563</v>
       </c>
       <c r="J159" s="1">
-        <v>0.80722348577800307</v>
+        <v>19.277651422199689</v>
       </c>
       <c r="K159" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.2">
@@ -5984,34 +5984,34 @@
         <v>2010</v>
       </c>
       <c r="B160" s="1">
-        <v>0.90929130411428283</v>
+        <v>9.0708695885717248</v>
       </c>
       <c r="C160" s="1">
-        <v>0.72070703267127911</v>
+        <v>27.929296732872093</v>
       </c>
       <c r="D160" s="1">
-        <v>0.98936953468338851</v>
+        <v>1.0630465316611413</v>
       </c>
       <c r="E160" s="1">
-        <v>9.0262622724384886E-2</v>
+        <v>90.973737727561513</v>
       </c>
       <c r="F160" s="1">
-        <v>0.36215115542800269</v>
+        <v>63.78488445719973</v>
       </c>
       <c r="G160" s="1">
-        <v>0.79635026541357046</v>
+        <v>20.364973458642957</v>
       </c>
       <c r="H160" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I160" s="1">
-        <v>0.42467272643224319</v>
+        <v>57.532727356775673</v>
       </c>
       <c r="J160" s="1">
-        <v>0.76148652925145022</v>
+        <v>23.851347074854974</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.2">
@@ -6019,34 +6019,34 @@
         <v>2011</v>
       </c>
       <c r="B161" s="1">
-        <v>0.91146562101119621</v>
+        <v>8.8534378988803795</v>
       </c>
       <c r="C161" s="1">
-        <v>0.72033724606132499</v>
+        <v>27.966275393867505</v>
       </c>
       <c r="D161" s="1">
-        <v>0.986650067575499</v>
+        <v>1.3349932424501065</v>
       </c>
       <c r="E161" s="1">
-        <v>9.2253724657423306E-2</v>
+        <v>90.774627534257661</v>
       </c>
       <c r="F161" s="1">
-        <v>0.36320136142890869</v>
+        <v>63.679863857109133</v>
       </c>
       <c r="G161" s="1">
-        <v>0.79373034133937215</v>
+        <v>20.626965866062786</v>
       </c>
       <c r="H161" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I161" s="1">
-        <v>0.40838444812976504</v>
+        <v>59.161555187023509</v>
       </c>
       <c r="J161" s="1">
-        <v>0.75531367017463746</v>
+        <v>24.468632982536249</v>
       </c>
       <c r="K161" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.2">
@@ -6054,34 +6054,34 @@
         <v>2012</v>
       </c>
       <c r="B162" s="1">
-        <v>0.9087041479536877</v>
+        <v>9.1295852046312351</v>
       </c>
       <c r="C162" s="1">
-        <v>0.7158756884215719</v>
+        <v>28.412431157842811</v>
       </c>
       <c r="D162" s="1">
-        <v>0.98511818179955513</v>
+        <v>1.4881818200444945</v>
       </c>
       <c r="E162" s="1">
-        <v>9.2691411979801616E-2</v>
+        <v>90.730858802019839</v>
       </c>
       <c r="F162" s="1">
-        <v>0.36033342667903634</v>
+        <v>63.966657332096375</v>
       </c>
       <c r="G162" s="1">
-        <v>0.79054593970017517</v>
+        <v>20.945406029982482</v>
       </c>
       <c r="H162" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I162" s="1">
-        <v>0.42808472098296341</v>
+        <v>57.191527901703665</v>
       </c>
       <c r="J162" s="1">
-        <v>0.7620658070373989</v>
+        <v>23.793419296260112</v>
       </c>
       <c r="K162" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.2">
@@ -6089,34 +6089,34 @@
         <v>2013</v>
       </c>
       <c r="B163" s="1">
-        <v>0.90551598703264535</v>
+        <v>9.4484012967354634</v>
       </c>
       <c r="C163" s="1">
-        <v>0.7081791879357906</v>
+        <v>29.182081206420946</v>
       </c>
       <c r="D163" s="1">
-        <v>0.98752754151078481</v>
+        <v>1.2472458489215195</v>
       </c>
       <c r="E163" s="1">
-        <v>8.9504671719578585E-2</v>
+        <v>91.049532828042146</v>
       </c>
       <c r="F163" s="1">
-        <v>0.36064311020823175</v>
+        <v>63.93568897917681</v>
       </c>
       <c r="G163" s="1">
-        <v>0.84338595387674031</v>
+        <v>15.661404612325965</v>
       </c>
       <c r="H163" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I163" s="1">
-        <v>0.42260255628017473</v>
+        <v>57.739744371982525</v>
       </c>
       <c r="J163" s="1">
-        <v>0.7402150001293184</v>
+        <v>25.978499987068172</v>
       </c>
       <c r="K163" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.2">
@@ -6124,34 +6124,34 @@
         <v>2014</v>
       </c>
       <c r="B164" s="1">
-        <v>0.90485621806993644</v>
+        <v>9.5143781930063653</v>
       </c>
       <c r="C164" s="1">
-        <v>0.70375909802917658</v>
+        <v>29.624090197082349</v>
       </c>
       <c r="D164" s="1">
-        <v>0.98749733684050411</v>
+        <v>1.2502663159495762</v>
       </c>
       <c r="E164" s="1">
-        <v>8.8063925052477593E-2</v>
+        <v>91.193607494752243</v>
       </c>
       <c r="F164" s="1">
-        <v>0.36339533290921006</v>
+        <v>63.660466709078989</v>
       </c>
       <c r="G164" s="1">
-        <v>0.83203289070919428</v>
+        <v>16.796710929080575</v>
       </c>
       <c r="H164" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I164" s="1">
-        <v>0.42552814397506039</v>
+        <v>57.447185602493953</v>
       </c>
       <c r="J164" s="1">
-        <v>0.74200090421129905</v>
+        <v>25.799909578870089</v>
       </c>
       <c r="K164" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.2">
@@ -6159,34 +6159,34 @@
         <v>2015</v>
       </c>
       <c r="B165" s="1">
-        <v>0.90394188241631368</v>
+        <v>9.6058117583686258</v>
       </c>
       <c r="C165" s="1">
-        <v>0.70287943391465191</v>
+        <v>29.712056608534805</v>
       </c>
       <c r="D165" s="1">
-        <v>0.98677482551733886</v>
+        <v>1.3225174482661104</v>
       </c>
       <c r="E165" s="1">
-        <v>8.8410547135578679E-2</v>
+        <v>91.158945286442133</v>
       </c>
       <c r="F165" s="1">
-        <v>0.3659652251654219</v>
+        <v>63.403477483457813</v>
       </c>
       <c r="G165" s="1">
-        <v>0.82051153118366194</v>
+        <v>17.948846881633816</v>
       </c>
       <c r="H165" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I165" s="1">
-        <v>0.4293491207847332</v>
+        <v>57.065087921526683</v>
       </c>
       <c r="J165" s="1">
-        <v>0.73956513583779993</v>
+        <v>26.043486416220013</v>
       </c>
       <c r="K165" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>